<commit_message>
20250924 - Camel case all name, fixed some padding for table row
</commit_message>
<xml_diff>
--- a/assets/score/bxb-template.xlsx
+++ b/assets/score/bxb-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PWRCh\OneDrive\Desktop\BatuuScoring\assets\score\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F2E3A3-D57E-4642-8E72-02E7DE5B122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089E2598-9D40-4082-A68C-E66F5B93EC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{7F520E0E-A91E-45B5-A85D-62EFB1C3D427}"/>
   </bookViews>
@@ -365,12 +365,6 @@
     <t>Ahmad Abid Adam</t>
   </si>
   <si>
-    <t>Ahmed mohammed khaled alareqi</t>
-  </si>
-  <si>
-    <t>AIMAN HAKEEMI BIN AWANG SUPIAN</t>
-  </si>
-  <si>
     <t>Ali Umar</t>
   </si>
   <si>
@@ -383,9 +377,6 @@
     <t>Amanda Lee Mun Yee</t>
   </si>
   <si>
-    <t>Amani</t>
-  </si>
-  <si>
     <t>Amirul</t>
   </si>
   <si>
@@ -398,12 +389,6 @@
     <t>Ang Yue</t>
   </si>
   <si>
-    <t>Arif Rasydan bin Abdul Rauf</t>
-  </si>
-  <si>
-    <t>Asfaq luthfiya</t>
-  </si>
-  <si>
     <t>Benjamin Chuah Xiao Xun</t>
   </si>
   <si>
@@ -431,9 +416,6 @@
     <t>Chan Zi Yue</t>
   </si>
   <si>
-    <t>CHANG CHING YET</t>
-  </si>
-  <si>
     <t>Charlotte Amanda Gan Sveet Ting</t>
   </si>
   <si>
@@ -461,9 +443,6 @@
     <t>Choo Hong Kai</t>
   </si>
   <si>
-    <t>Choo Wen hui</t>
-  </si>
-  <si>
     <t>Chow Ee Ling Zoe</t>
   </si>
   <si>
@@ -485,9 +464,6 @@
     <t>Daryl Lim Wei Sien</t>
   </si>
   <si>
-    <t>Denise</t>
-  </si>
-  <si>
     <t>Denver Wong Der-Qi</t>
   </si>
   <si>
@@ -506,9 +482,6 @@
     <t>Ethan Khoo Kay Shing</t>
   </si>
   <si>
-    <t>Ethan tan bo wen</t>
-  </si>
-  <si>
     <t>Eugene Chin Hwa En</t>
   </si>
   <si>
@@ -530,21 +503,12 @@
     <t>Fun Keng Soon</t>
   </si>
   <si>
-    <t>Gan Hoong liang</t>
-  </si>
-  <si>
     <t>Gwen Koh Ting Zhi</t>
   </si>
   <si>
-    <t>HAZIM MUSYRIF BIN SAIFUDDIN</t>
-  </si>
-  <si>
     <t>Henry Choo Wen Hui</t>
   </si>
   <si>
-    <t>IMAN DANIAL BIN FAIRUL AZRAI</t>
-  </si>
-  <si>
     <t>Irsyad Izac</t>
   </si>
   <si>
@@ -605,9 +569,6 @@
     <t>Justin Peck Qing En</t>
   </si>
   <si>
-    <t>karly tan kai yen</t>
-  </si>
-  <si>
     <t>Katherina Izreen</t>
   </si>
   <si>
@@ -617,18 +578,12 @@
     <t>Kenton Ng</t>
   </si>
   <si>
-    <t>KIANG XIN YIN</t>
-  </si>
-  <si>
     <t>Kimberly Ho Mei Yi</t>
   </si>
   <si>
     <t>Kong Zheng Yang</t>
   </si>
   <si>
-    <t>LANISHA ANUSRI A/P SARAVANAN</t>
-  </si>
-  <si>
     <t>Lavender Ling Wei Huey</t>
   </si>
   <si>
@@ -656,9 +611,6 @@
     <t>Lexus Goh Ka Shing</t>
   </si>
   <si>
-    <t>Lian YaoMing</t>
-  </si>
-  <si>
     <t>Liew Heng Jian</t>
   </si>
   <si>
@@ -668,9 +620,6 @@
     <t>Lim Jian Tao</t>
   </si>
   <si>
-    <t>LIM JUN</t>
-  </si>
-  <si>
     <t>Lim Jun Hong</t>
   </si>
   <si>
@@ -704,9 +653,6 @@
     <t>Luo Kian Yang</t>
   </si>
   <si>
-    <t>MALCOLM MU JENN BANG</t>
-  </si>
-  <si>
     <t>Matthew Thong</t>
   </si>
   <si>
@@ -758,12 +704,6 @@
     <t>Nie Naik Wei Qin</t>
   </si>
   <si>
-    <t>Nik Zulhariz bin Nik Fuaad</t>
-  </si>
-  <si>
-    <t>NUR UMIRAH BINTI MAT YUSNI</t>
-  </si>
-  <si>
     <t>Nurul Farhana Azman</t>
   </si>
   <si>
@@ -791,9 +731,6 @@
     <t>Raslan Abdul Rahman</t>
   </si>
   <si>
-    <t>RIKKI WEN</t>
-  </si>
-  <si>
     <t>Ronald Lee Yit Yuan</t>
   </si>
   <si>
@@ -815,9 +752,6 @@
     <t>San Haw Nan</t>
   </si>
   <si>
-    <t>Shahrizad bin Shazuddin</t>
-  </si>
-  <si>
     <t>Sharifah Farzana Binti Syed Alfarly</t>
   </si>
   <si>
@@ -878,9 +812,6 @@
     <t>Timothy Tan Ming Yang</t>
   </si>
   <si>
-    <t>Trisha Tiffenie tan</t>
-  </si>
-  <si>
     <t>Tristan Alexander Pheh Xin Jian</t>
   </si>
   <si>
@@ -932,9 +863,6 @@
     <t>Yap Kee Sheng</t>
   </si>
   <si>
-    <t>Yee Kah hao</t>
-  </si>
-  <si>
     <t>Yeo Aik Cheng</t>
   </si>
   <si>
@@ -956,10 +884,82 @@
     <t>Yusuf Hamdani Bin Abd Manan</t>
   </si>
   <si>
-    <t>Zachary Matthew alabaster</t>
-  </si>
-  <si>
     <t>Zachary Ng Yie-Jie</t>
+  </si>
+  <si>
+    <t>Ahmed Mohammed Khaled Alareqi</t>
+  </si>
+  <si>
+    <t>Aiman Hakeemi Bin Awang Supian</t>
+  </si>
+  <si>
+    <t>Arif Rasydan Bin Abdul Rauf</t>
+  </si>
+  <si>
+    <t>Asfaq Luthfiya</t>
+  </si>
+  <si>
+    <t>Chang Ching Yet</t>
+  </si>
+  <si>
+    <t>Choo Wen Hui</t>
+  </si>
+  <si>
+    <t>Denise Wong</t>
+  </si>
+  <si>
+    <t>Ethan Tan Bo Wen</t>
+  </si>
+  <si>
+    <t>Gan Hoong Liang</t>
+  </si>
+  <si>
+    <t>Hazim Musyrif Bin Saifuddin</t>
+  </si>
+  <si>
+    <t>Iman Danial Bin Fairul Azrai</t>
+  </si>
+  <si>
+    <t>Izzah Amani</t>
+  </si>
+  <si>
+    <t>Karly Tan Kai Yen</t>
+  </si>
+  <si>
+    <t>Kiang Xin Yin</t>
+  </si>
+  <si>
+    <t>Lanisha Anusri A/P Saravanan</t>
+  </si>
+  <si>
+    <t>Lian Yaoming</t>
+  </si>
+  <si>
+    <t>Lim Jun</t>
+  </si>
+  <si>
+    <t>Malcolm Mu Jenn Bang</t>
+  </si>
+  <si>
+    <t>Nik Zulhariz Bin Nik Fuaad</t>
+  </si>
+  <si>
+    <t>Nur Umirah Binti Mat Yusni</t>
+  </si>
+  <si>
+    <t>Rikki Wen</t>
+  </si>
+  <si>
+    <t>Shahrizad Bin Shazuddin</t>
+  </si>
+  <si>
+    <t>Trisha Tiffenie Tan</t>
+  </si>
+  <si>
+    <t>Yee Kah Hao</t>
+  </si>
+  <si>
+    <t>Zachary Matthew Alabaster</t>
   </si>
 </sst>
 </file>
@@ -1442,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FD4630-A43E-4101-88FC-4337AD741BC4}">
   <dimension ref="A1:CX207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:AA207"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="9" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>283</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="10" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>284</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -2080,7 +2080,7 @@
     </row>
     <row r="11" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="12" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="13" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -2182,7 +2182,7 @@
     </row>
     <row r="14" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="15" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="16" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="17" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="18" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="19" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>285</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="20" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>286</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="21" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="22" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="23" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="24" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
@@ -2556,7 +2556,7 @@
     </row>
     <row r="25" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="26" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="27" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="28" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="29" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="30" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>287</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
@@ -2760,7 +2760,7 @@
     </row>
     <row r="31" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="32" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="33" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="34" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="35" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="36" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
@@ -2964,7 +2964,7 @@
     </row>
     <row r="37" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="38" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="39" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="40" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>288</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="41" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
@@ -3134,7 +3134,7 @@
     </row>
     <row r="42" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
@@ -3168,7 +3168,7 @@
     </row>
     <row r="43" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
@@ -3202,7 +3202,7 @@
     </row>
     <row r="44" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="45" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="46" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="47" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="48" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>289</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="49" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
@@ -3406,7 +3406,7 @@
     </row>
     <row r="50" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="51" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
@@ -3474,7 +3474,7 @@
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
@@ -3508,7 +3508,7 @@
     </row>
     <row r="53" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
@@ -3542,7 +3542,7 @@
     </row>
     <row r="54" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
@@ -3576,7 +3576,7 @@
     </row>
     <row r="55" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>290</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="56" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="57" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
@@ -3678,7 +3678,7 @@
     </row>
     <row r="58" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
@@ -3712,7 +3712,7 @@
     </row>
     <row r="59" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="60" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
@@ -3780,7 +3780,7 @@
     </row>
     <row r="61" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
@@ -3814,7 +3814,7 @@
     </row>
     <row r="62" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="63" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>163</v>
+        <v>291</v>
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
@@ -3882,7 +3882,7 @@
     </row>
     <row r="64" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
@@ -3916,7 +3916,7 @@
     </row>
     <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>165</v>
+        <v>292</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="66" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
@@ -3984,7 +3984,7 @@
     </row>
     <row r="67" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B130" si="1">SUM(C67:CX67)</f>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="68" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B68">
         <f t="shared" si="1"/>
@@ -4052,7 +4052,7 @@
     </row>
     <row r="69" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B69">
         <f t="shared" si="1"/>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="70" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="71" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>294</v>
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
@@ -4154,7 +4154,7 @@
     </row>
     <row r="72" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B72">
         <f t="shared" si="1"/>
@@ -4188,7 +4188,7 @@
     </row>
     <row r="73" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B73">
         <f t="shared" si="1"/>
@@ -4222,7 +4222,7 @@
     </row>
     <row r="74" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B74">
         <f t="shared" si="1"/>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="75" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B75">
         <f t="shared" si="1"/>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="76" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B76">
         <f t="shared" si="1"/>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="77" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B77">
         <f t="shared" si="1"/>
@@ -4358,7 +4358,7 @@
     </row>
     <row r="78" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B78">
         <f t="shared" si="1"/>
@@ -4392,7 +4392,7 @@
     </row>
     <row r="79" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B79">
         <f t="shared" si="1"/>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="80" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
@@ -4460,7 +4460,7 @@
     </row>
     <row r="81" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="82" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
@@ -4528,7 +4528,7 @@
     </row>
     <row r="83" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B83">
         <f t="shared" si="1"/>
@@ -4562,7 +4562,7 @@
     </row>
     <row r="84" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B84">
         <f t="shared" si="1"/>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="85" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B85">
         <f t="shared" si="1"/>
@@ -4630,7 +4630,7 @@
     </row>
     <row r="86" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B86">
         <f t="shared" si="1"/>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="87" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B87">
         <f t="shared" si="1"/>
@@ -4698,7 +4698,7 @@
     </row>
     <row r="88" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B88">
         <f t="shared" si="1"/>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="89" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
-        <v>189</v>
+        <v>295</v>
       </c>
       <c r="B89">
         <f t="shared" si="1"/>
@@ -4766,7 +4766,7 @@
     </row>
     <row r="90" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B90">
         <f t="shared" si="1"/>
@@ -4800,7 +4800,7 @@
     </row>
     <row r="91" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B91">
         <f t="shared" si="1"/>
@@ -4834,7 +4834,7 @@
     </row>
     <row r="92" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="B92">
         <f t="shared" si="1"/>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="93" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>296</v>
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
@@ -4902,7 +4902,7 @@
     </row>
     <row r="94" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B94">
         <f t="shared" si="1"/>
@@ -4936,7 +4936,7 @@
     </row>
     <row r="95" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B95">
         <f t="shared" si="1"/>
@@ -4970,7 +4970,7 @@
     </row>
     <row r="96" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
-        <v>196</v>
+        <v>297</v>
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
@@ -5004,7 +5004,7 @@
     </row>
     <row r="97" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B97">
         <f t="shared" si="1"/>
@@ -5038,7 +5038,7 @@
     </row>
     <row r="98" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B98">
         <f t="shared" si="1"/>
@@ -5072,7 +5072,7 @@
     </row>
     <row r="99" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B99">
         <f t="shared" si="1"/>
@@ -5106,7 +5106,7 @@
     </row>
     <row r="100" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B100">
         <f t="shared" si="1"/>
@@ -5140,7 +5140,7 @@
     </row>
     <row r="101" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="B101">
         <f t="shared" si="1"/>
@@ -5174,7 +5174,7 @@
     </row>
     <row r="102" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="B102">
         <f t="shared" si="1"/>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="103" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B103">
         <f t="shared" si="1"/>
@@ -5242,7 +5242,7 @@
     </row>
     <row r="104" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B104">
         <f t="shared" si="1"/>
@@ -5276,7 +5276,7 @@
     </row>
     <row r="105" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="B105">
         <f t="shared" si="1"/>
@@ -5310,7 +5310,7 @@
     </row>
     <row r="106" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>298</v>
       </c>
       <c r="B106">
         <f t="shared" si="1"/>
@@ -5344,7 +5344,7 @@
     </row>
     <row r="107" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B107">
         <f t="shared" si="1"/>
@@ -5378,7 +5378,7 @@
     </row>
     <row r="108" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="B108">
         <f t="shared" si="1"/>
@@ -5412,7 +5412,7 @@
     </row>
     <row r="109" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="B109">
         <f t="shared" si="1"/>
@@ -5446,7 +5446,7 @@
     </row>
     <row r="110" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>299</v>
       </c>
       <c r="B110">
         <f t="shared" si="1"/>
@@ -5480,7 +5480,7 @@
     </row>
     <row r="111" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="B111">
         <f t="shared" si="1"/>
@@ -5514,7 +5514,7 @@
     </row>
     <row r="112" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="B112">
         <f t="shared" si="1"/>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="113" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="B113">
         <f t="shared" si="1"/>
@@ -5582,7 +5582,7 @@
     </row>
     <row r="114" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="B114">
         <f t="shared" si="1"/>
@@ -5616,7 +5616,7 @@
     </row>
     <row r="115" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="B115">
         <f t="shared" si="1"/>
@@ -5650,7 +5650,7 @@
     </row>
     <row r="116" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="B116">
         <f t="shared" si="1"/>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="117" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="B117">
         <f t="shared" si="1"/>
@@ -5718,7 +5718,7 @@
     </row>
     <row r="118" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="B118">
         <f t="shared" si="1"/>
@@ -5752,7 +5752,7 @@
     </row>
     <row r="119" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="B119">
         <f t="shared" si="1"/>
@@ -5786,7 +5786,7 @@
     </row>
     <row r="120" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="B120">
         <f t="shared" si="1"/>
@@ -5820,7 +5820,7 @@
     </row>
     <row r="121" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="B121">
         <f t="shared" si="1"/>
@@ -5854,7 +5854,7 @@
     </row>
     <row r="122" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
-        <v>222</v>
+        <v>300</v>
       </c>
       <c r="B122">
         <f t="shared" si="1"/>
@@ -5888,7 +5888,7 @@
     </row>
     <row r="123" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B123">
         <f t="shared" si="1"/>
@@ -5922,7 +5922,7 @@
     </row>
     <row r="124" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="B124">
         <f t="shared" si="1"/>
@@ -5956,7 +5956,7 @@
     </row>
     <row r="125" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="B125">
         <f t="shared" si="1"/>
@@ -5990,7 +5990,7 @@
     </row>
     <row r="126" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B126">
         <f t="shared" si="1"/>
@@ -6024,7 +6024,7 @@
     </row>
     <row r="127" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="B127">
         <f t="shared" si="1"/>
@@ -6058,7 +6058,7 @@
     </row>
     <row r="128" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="B128">
         <f t="shared" si="1"/>
@@ -6092,7 +6092,7 @@
     </row>
     <row r="129" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="B129">
         <f t="shared" si="1"/>
@@ -6126,7 +6126,7 @@
     </row>
     <row r="130" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="B130">
         <f t="shared" si="1"/>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="131" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="B131">
         <f t="shared" ref="B131:B194" si="2">SUM(C131:CX131)</f>
@@ -6194,7 +6194,7 @@
     </row>
     <row r="132" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="B132">
         <f t="shared" si="2"/>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="133" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="B133">
         <f t="shared" si="2"/>
@@ -6262,7 +6262,7 @@
     </row>
     <row r="134" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="B134">
         <f t="shared" si="2"/>
@@ -6296,7 +6296,7 @@
     </row>
     <row r="135" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="B135">
         <f t="shared" si="2"/>
@@ -6330,7 +6330,7 @@
     </row>
     <row r="136" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="B136">
         <f t="shared" si="2"/>
@@ -6364,7 +6364,7 @@
     </row>
     <row r="137" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="B137">
         <f t="shared" si="2"/>
@@ -6398,7 +6398,7 @@
     </row>
     <row r="138" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="B138">
         <f t="shared" si="2"/>
@@ -6432,7 +6432,7 @@
     </row>
     <row r="139" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="B139">
         <f t="shared" si="2"/>
@@ -6466,7 +6466,7 @@
     </row>
     <row r="140" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
-        <v>240</v>
+        <v>301</v>
       </c>
       <c r="B140">
         <f t="shared" si="2"/>
@@ -6500,7 +6500,7 @@
     </row>
     <row r="141" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
-        <v>241</v>
+        <v>302</v>
       </c>
       <c r="B141">
         <f t="shared" si="2"/>
@@ -6534,7 +6534,7 @@
     </row>
     <row r="142" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="B142">
         <f t="shared" si="2"/>
@@ -6568,7 +6568,7 @@
     </row>
     <row r="143" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B143">
         <f t="shared" si="2"/>
@@ -6602,7 +6602,7 @@
     </row>
     <row r="144" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B144">
         <f t="shared" si="2"/>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="145" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B145">
         <f t="shared" si="2"/>
@@ -6670,7 +6670,7 @@
     </row>
     <row r="146" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B146">
         <f t="shared" si="2"/>
@@ -6704,7 +6704,7 @@
     </row>
     <row r="147" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="B147">
         <f t="shared" si="2"/>
@@ -6738,7 +6738,7 @@
     </row>
     <row r="148" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="B148">
         <f t="shared" si="2"/>
@@ -6772,7 +6772,7 @@
     </row>
     <row r="149" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B149">
         <f t="shared" si="2"/>
@@ -6806,7 +6806,7 @@
     </row>
     <row r="150" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B150">
         <f t="shared" si="2"/>
@@ -6840,7 +6840,7 @@
     </row>
     <row r="151" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
-        <v>251</v>
+        <v>303</v>
       </c>
       <c r="B151">
         <f t="shared" si="2"/>
@@ -6874,7 +6874,7 @@
     </row>
     <row r="152" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="B152">
         <f t="shared" si="2"/>
@@ -6908,7 +6908,7 @@
     </row>
     <row r="153" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="B153">
         <f t="shared" si="2"/>
@@ -6942,7 +6942,7 @@
     </row>
     <row r="154" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="B154">
         <f t="shared" si="2"/>
@@ -6976,7 +6976,7 @@
     </row>
     <row r="155" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="B155">
         <f t="shared" si="2"/>
@@ -7010,7 +7010,7 @@
     </row>
     <row r="156" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="B156">
         <f t="shared" si="2"/>
@@ -7044,7 +7044,7 @@
     </row>
     <row r="157" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="B157">
         <f t="shared" si="2"/>
@@ -7078,7 +7078,7 @@
     </row>
     <row r="158" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="B158">
         <f t="shared" si="2"/>
@@ -7112,7 +7112,7 @@
     </row>
     <row r="159" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="B159">
         <f t="shared" si="2"/>
@@ -7146,7 +7146,7 @@
     </row>
     <row r="160" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="B160">
         <f t="shared" si="2"/>
@@ -7180,7 +7180,7 @@
     </row>
     <row r="161" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="B161">
         <f t="shared" si="2"/>
@@ -7214,7 +7214,7 @@
     </row>
     <row r="162" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
       <c r="B162">
         <f t="shared" si="2"/>
@@ -7248,7 +7248,7 @@
     </row>
     <row r="163" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="B163">
         <f t="shared" si="2"/>
@@ -7282,7 +7282,7 @@
     </row>
     <row r="164" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="B164">
         <f t="shared" si="2"/>
@@ -7316,7 +7316,7 @@
     </row>
     <row r="165" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="B165">
         <f t="shared" si="2"/>
@@ -7350,7 +7350,7 @@
     </row>
     <row r="166" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="B166">
         <f t="shared" si="2"/>
@@ -7384,7 +7384,7 @@
     </row>
     <row r="167" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="B167">
         <f t="shared" si="2"/>
@@ -7418,7 +7418,7 @@
     </row>
     <row r="168" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="B168">
         <f t="shared" si="2"/>
@@ -7452,7 +7452,7 @@
     </row>
     <row r="169" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A169" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="B169">
         <f t="shared" si="2"/>
@@ -7486,7 +7486,7 @@
     </row>
     <row r="170" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A170" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="B170">
         <f t="shared" si="2"/>
@@ -7520,7 +7520,7 @@
     </row>
     <row r="171" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A171" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="B171">
         <f t="shared" si="2"/>
@@ -7554,7 +7554,7 @@
     </row>
     <row r="172" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A172" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="B172">
         <f t="shared" si="2"/>
@@ -7588,7 +7588,7 @@
     </row>
     <row r="173" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A173" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="B173">
         <f t="shared" si="2"/>
@@ -7622,7 +7622,7 @@
     </row>
     <row r="174" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A174" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="B174">
         <f t="shared" si="2"/>
@@ -7656,7 +7656,7 @@
     </row>
     <row r="175" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A175" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
       <c r="B175">
         <f t="shared" si="2"/>
@@ -7690,7 +7690,7 @@
     </row>
     <row r="176" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A176" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="B176">
         <f t="shared" si="2"/>
@@ -7724,7 +7724,7 @@
     </row>
     <row r="177" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A177" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="B177">
         <f t="shared" si="2"/>
@@ -7758,7 +7758,7 @@
     </row>
     <row r="178" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A178" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="B178">
         <f t="shared" si="2"/>
@@ -7792,7 +7792,7 @@
     </row>
     <row r="179" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A179" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
       <c r="B179">
         <f t="shared" si="2"/>
@@ -7826,7 +7826,7 @@
     </row>
     <row r="180" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A180" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="B180">
         <f t="shared" si="2"/>
@@ -7860,7 +7860,7 @@
     </row>
     <row r="181" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A181" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="B181">
         <f t="shared" si="2"/>
@@ -7894,7 +7894,7 @@
     </row>
     <row r="182" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A182" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="B182">
         <f t="shared" si="2"/>
@@ -7928,7 +7928,7 @@
     </row>
     <row r="183" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A183" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="B183">
         <f t="shared" si="2"/>
@@ -7962,7 +7962,7 @@
     </row>
     <row r="184" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="B184">
         <f t="shared" si="2"/>
@@ -7996,7 +7996,7 @@
     </row>
     <row r="185" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A185" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="B185">
         <f t="shared" si="2"/>
@@ -8030,7 +8030,7 @@
     </row>
     <row r="186" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A186" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="B186">
         <f t="shared" si="2"/>
@@ -8064,7 +8064,7 @@
     </row>
     <row r="187" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A187" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="B187">
         <f t="shared" si="2"/>
@@ -8098,7 +8098,7 @@
     </row>
     <row r="188" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A188" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="B188">
         <f t="shared" si="2"/>
@@ -8132,7 +8132,7 @@
     </row>
     <row r="189" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A189" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="B189">
         <f t="shared" si="2"/>
@@ -8166,7 +8166,7 @@
     </row>
     <row r="190" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A190" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="B190">
         <f t="shared" si="2"/>
@@ -8200,7 +8200,7 @@
     </row>
     <row r="191" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A191" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="B191">
         <f t="shared" si="2"/>
@@ -8234,7 +8234,7 @@
     </row>
     <row r="192" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A192" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="B192">
         <f t="shared" si="2"/>
@@ -8268,7 +8268,7 @@
     </row>
     <row r="193" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A193" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="B193">
         <f t="shared" si="2"/>
@@ -8302,7 +8302,7 @@
     </row>
     <row r="194" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A194" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="B194">
         <f t="shared" si="2"/>
@@ -8336,7 +8336,7 @@
     </row>
     <row r="195" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A195" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="B195">
         <f t="shared" ref="B195:B207" si="3">SUM(C195:CX195)</f>
@@ -8370,7 +8370,7 @@
     </row>
     <row r="196" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A196" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="B196">
         <f t="shared" si="3"/>
@@ -8404,7 +8404,7 @@
     </row>
     <row r="197" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A197" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="B197">
         <f t="shared" si="3"/>
@@ -8438,7 +8438,7 @@
     </row>
     <row r="198" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="B198">
         <f t="shared" si="3"/>
@@ -8472,7 +8472,7 @@
     </row>
     <row r="199" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A199" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="B199">
         <f t="shared" si="3"/>
@@ -8506,7 +8506,7 @@
     </row>
     <row r="200" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A200" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="B200">
         <f t="shared" si="3"/>
@@ -8540,7 +8540,7 @@
     </row>
     <row r="201" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A201" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="B201">
         <f t="shared" si="3"/>
@@ -8574,7 +8574,7 @@
     </row>
     <row r="202" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A202" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="B202">
         <f t="shared" si="3"/>
@@ -8608,7 +8608,7 @@
     </row>
     <row r="203" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A203" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="B203">
         <f t="shared" si="3"/>
@@ -8642,7 +8642,7 @@
     </row>
     <row r="204" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A204" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="B204">
         <f t="shared" si="3"/>
@@ -8676,7 +8676,7 @@
     </row>
     <row r="205" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A205" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="B205">
         <f t="shared" si="3"/>
@@ -8710,7 +8710,7 @@
     </row>
     <row r="206" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A206" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B206">
         <f t="shared" si="3"/>
@@ -8744,7 +8744,7 @@
     </row>
     <row r="207" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A207" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="B207">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
20250925 - Added entries of people and realign scores
</commit_message>
<xml_diff>
--- a/assets/score/bxb-template.xlsx
+++ b/assets/score/bxb-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genryu\Desktop\bxbscore\assets\score\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PWRCh\OneDrive\Desktop\gitproject\bxbscore\assets\score\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D99477-50A3-4FA5-ADBF-090B73C95DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8E15F9-E2C3-4BAA-87B5-27421E1D81A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7F520E0E-A91E-45B5-A85D-62EFB1C3D427}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{7F520E0E-A91E-45B5-A85D-62EFB1C3D427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="318">
   <si>
     <t>Participant Name</t>
   </si>
@@ -395,9 +395,6 @@
     <t>Benno</t>
   </si>
   <si>
-    <t>Brendon Chew Whei Jin</t>
-  </si>
-  <si>
     <t>Brennan Shin</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
     <t>Chu Jia Chen</t>
   </si>
   <si>
-    <t>Chua Xue Yi</t>
-  </si>
-  <si>
     <t>Chun Sin Ling</t>
   </si>
   <si>
@@ -479,9 +473,6 @@
     <t>Esther Ooi Lay Tsim</t>
   </si>
   <si>
-    <t>Ethan Khoo Kay Shing</t>
-  </si>
-  <si>
     <t>Eugene Chin Hwa En</t>
   </si>
   <si>
@@ -491,9 +482,6 @@
     <t>Felix Chai Yueh Hong</t>
   </si>
   <si>
-    <t>Fern Chong</t>
-  </si>
-  <si>
     <t>Foo Joo Wee</t>
   </si>
   <si>
@@ -581,9 +569,6 @@
     <t>Kimberly Ho Mei Yi</t>
   </si>
   <si>
-    <t>Kong Zheng Yang</t>
-  </si>
-  <si>
     <t>Lavender Ling Wei Huey</t>
   </si>
   <si>
@@ -680,9 +665,6 @@
     <t>Ng Hong Ming</t>
   </si>
   <si>
-    <t>Ng Jing En</t>
-  </si>
-  <si>
     <t>Ng Wan Wen</t>
   </si>
   <si>
@@ -782,9 +764,6 @@
     <t>Sudais Bin Mohd Ferhard</t>
   </si>
   <si>
-    <t>Syahryl Bin Mohamad Serkawini</t>
-  </si>
-  <si>
     <t>Syed Kamal Azriff Bin Syed Amran</t>
   </si>
   <si>
@@ -960,13 +939,64 @@
   </si>
   <si>
     <t>Zachary Matthew Alabaster</t>
+  </si>
+  <si>
+    <t>Charmaine Lim Xin Le</t>
+  </si>
+  <si>
+    <t>Cheong Wei Shin Samuel</t>
+  </si>
+  <si>
+    <t>Danial Imran</t>
+  </si>
+  <si>
+    <t>Khairul Irfan Bin Khairul Hamidi</t>
+  </si>
+  <si>
+    <t>Liew Qi Yan (Terrence)</t>
+  </si>
+  <si>
+    <t>Marilyn Tee Yan Zyn</t>
+  </si>
+  <si>
+    <t>Ng Shan-Zi</t>
+  </si>
+  <si>
+    <t>Arif Fikri Bin Othman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brendon Chew Whei Jin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chua Xue Yi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethan Khoo Kay Shing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fern Chong </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kong Zheng Yang </t>
+  </si>
+  <si>
+    <t>Low Jin Shen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ng Jing En </t>
+  </si>
+  <si>
+    <t>Ong Kuok Tjun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syahryl Bin Mohamad Serkawini </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -979,6 +1009,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1073,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1108,6 +1143,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1449,25 +1493,25 @@
       <selection activeCell="C2" sqref="C2:AA217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="36" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="40" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="52" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="61" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="64" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="77" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="86" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="89" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="90" max="102" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="27" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="36" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="52" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="53" max="61" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="62" max="64" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="65" max="77" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="78" max="86" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="87" max="89" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="90" max="102" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1775,8 +1819,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="13" t="s">
         <v>102</v>
       </c>
       <c r="B2">
@@ -1819,8 +1863,8 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
     </row>
-    <row r="3" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
         <v>103</v>
       </c>
       <c r="B3">
@@ -1869,8 +1913,8 @@
       <c r="Z3" s="9"/>
       <c r="AA3" s="9"/>
     </row>
-    <row r="4" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B4">
@@ -1913,8 +1957,8 @@
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
     </row>
-    <row r="5" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="14" t="s">
         <v>105</v>
       </c>
       <c r="B5">
@@ -1965,8 +2009,8 @@
       <c r="Z5" s="9"/>
       <c r="AA5" s="9"/>
     </row>
-    <row r="6" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="14" t="s">
         <v>106</v>
       </c>
       <c r="B6">
@@ -2021,8 +2065,8 @@
       </c>
       <c r="AA6" s="9"/>
     </row>
-    <row r="7" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B7">
@@ -2055,8 +2099,8 @@
       <c r="Z7" s="9"/>
       <c r="AA7" s="9"/>
     </row>
-    <row r="8" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B8">
@@ -2113,9 +2157,9 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
     </row>
-    <row r="9" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>283</v>
+    <row r="9" spans="1:102" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="14" t="s">
+        <v>276</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -2165,9 +2209,9 @@
       <c r="Z9" s="9"/>
       <c r="AA9" s="9"/>
     </row>
-    <row r="10" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>284</v>
+    <row r="10" spans="1:102" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="14" t="s">
+        <v>277</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -2211,8 +2255,8 @@
       <c r="Z10" s="9"/>
       <c r="AA10" s="9"/>
     </row>
-    <row r="11" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B11">
@@ -2263,8 +2307,8 @@
       <c r="Z11" s="9"/>
       <c r="AA11" s="9"/>
     </row>
-    <row r="12" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="14" t="s">
         <v>110</v>
       </c>
       <c r="B12">
@@ -2305,8 +2349,8 @@
       <c r="Z12" s="9"/>
       <c r="AA12" s="9"/>
     </row>
-    <row r="13" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B13">
@@ -2339,8 +2383,8 @@
       <c r="Z13" s="9"/>
       <c r="AA13" s="9"/>
     </row>
-    <row r="14" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="14" t="s">
         <v>112</v>
       </c>
       <c r="B14">
@@ -2385,8 +2429,8 @@
       </c>
       <c r="AA14" s="9"/>
     </row>
-    <row r="15" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="14" t="s">
         <v>113</v>
       </c>
       <c r="B15">
@@ -2419,8 +2463,8 @@
       <c r="Z15" s="9"/>
       <c r="AA15" s="9"/>
     </row>
-    <row r="16" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="14" t="s">
         <v>114</v>
       </c>
       <c r="B16">
@@ -2453,8 +2497,8 @@
       <c r="Z16" s="9"/>
       <c r="AA16" s="9"/>
     </row>
-    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="14" t="s">
         <v>115</v>
       </c>
       <c r="B17">
@@ -2487,8 +2531,8 @@
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
     </row>
-    <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="14" t="s">
         <v>116</v>
       </c>
       <c r="B18">
@@ -2543,9 +2587,9 @@
       </c>
       <c r="AA18" s="9"/>
     </row>
-    <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>285</v>
+    <row r="19" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="14" t="s">
+        <v>308</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -2587,9 +2631,9 @@
       <c r="Z19" s="9"/>
       <c r="AA19" s="9"/>
     </row>
-    <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>286</v>
+    <row r="20" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="14" t="s">
+        <v>278</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -2637,9 +2681,9 @@
       <c r="Z20" s="9"/>
       <c r="AA20" s="9"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>117</v>
+    <row r="21" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="14" t="s">
+        <v>279</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -2671,9 +2715,9 @@
       <c r="Z21" s="9"/>
       <c r="AA21" s="9"/>
     </row>
-    <row r="22" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>118</v>
+    <row r="22" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
@@ -2705,9 +2749,9 @@
       <c r="Z22" s="9"/>
       <c r="AA22" s="9"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>119</v>
+    <row r="23" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -2739,9 +2783,9 @@
       <c r="Z23" s="9"/>
       <c r="AA23" s="9"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>120</v>
+    <row r="24" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="14" t="s">
+        <v>309</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
@@ -2791,9 +2835,9 @@
       <c r="Z24" s="9"/>
       <c r="AA24" s="9"/>
     </row>
-    <row r="25" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>121</v>
+    <row r="25" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
@@ -2825,9 +2869,9 @@
       <c r="Z25" s="9"/>
       <c r="AA25" s="9"/>
     </row>
-    <row r="26" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>122</v>
+    <row r="26" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
@@ -2883,9 +2927,9 @@
       <c r="Z26" s="9"/>
       <c r="AA26" s="9"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>123</v>
+    <row r="27" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
@@ -2937,9 +2981,9 @@
       <c r="Z27" s="9"/>
       <c r="AA27" s="9"/>
     </row>
-    <row r="28" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>124</v>
+    <row r="28" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="14" t="s">
+        <v>122</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
@@ -2983,9 +3027,9 @@
       <c r="Z28" s="9"/>
       <c r="AA28" s="9"/>
     </row>
-    <row r="29" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>125</v>
+    <row r="29" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
@@ -3017,9 +3061,9 @@
       <c r="Z29" s="9"/>
       <c r="AA29" s="9"/>
     </row>
-    <row r="30" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>287</v>
+    <row r="30" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
@@ -3051,9 +3095,9 @@
       <c r="Z30" s="9"/>
       <c r="AA30" s="9"/>
     </row>
-    <row r="31" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>126</v>
+    <row r="31" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="14" t="s">
+        <v>280</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
@@ -3085,9 +3129,9 @@
       <c r="Z31" s="9"/>
       <c r="AA31" s="9"/>
     </row>
-    <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>127</v>
+    <row r="32" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
@@ -3125,9 +3169,9 @@
       <c r="Z32" s="9"/>
       <c r="AA32" s="9"/>
     </row>
-    <row r="33" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>128</v>
+    <row r="33" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="14" t="s">
+        <v>301</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
@@ -3159,9 +3203,9 @@
       <c r="Z33" s="9"/>
       <c r="AA33" s="9"/>
     </row>
-    <row r="34" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>129</v>
+    <row r="34" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
@@ -3193,9 +3237,9 @@
       <c r="Z34" s="9"/>
       <c r="AA34" s="9"/>
     </row>
-    <row r="35" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>130</v>
+    <row r="35" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
@@ -3239,13 +3283,13 @@
       <c r="Z35" s="9"/>
       <c r="AA35" s="9"/>
     </row>
-    <row r="36" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>131</v>
+    <row r="36" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="14" t="s">
+        <v>128</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="8"/>
@@ -3260,7 +3304,9 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
-      <c r="P36" s="9"/>
+      <c r="P36" s="11">
+        <v>1</v>
+      </c>
       <c r="Q36" s="11">
         <v>1</v>
       </c>
@@ -3285,9 +3331,9 @@
       <c r="Z36" s="9"/>
       <c r="AA36" s="9"/>
     </row>
-    <row r="37" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>132</v>
+    <row r="37" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="14" t="s">
+        <v>302</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
@@ -3341,9 +3387,9 @@
       <c r="Z37" s="9"/>
       <c r="AA37" s="9"/>
     </row>
-    <row r="38" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>133</v>
+    <row r="38" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
@@ -3393,9 +3439,9 @@
       </c>
       <c r="AA38" s="9"/>
     </row>
-    <row r="39" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>134</v>
+    <row r="39" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
@@ -3453,13 +3499,13 @@
       <c r="Z39" s="9"/>
       <c r="AA39" s="9"/>
     </row>
-    <row r="40" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>288</v>
+    <row r="40" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C40" s="6">
         <v>1</v>
@@ -3492,22 +3538,34 @@
       <c r="O40" s="7">
         <v>1</v>
       </c>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
+      <c r="P40" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="11">
+        <v>1</v>
+      </c>
       <c r="R40" s="9"/>
       <c r="S40" s="9"/>
-      <c r="T40" s="9"/>
+      <c r="T40" s="11">
+        <v>1</v>
+      </c>
       <c r="U40" s="9"/>
-      <c r="V40" s="9"/>
+      <c r="V40" s="11">
+        <v>1</v>
+      </c>
       <c r="W40" s="9"/>
       <c r="X40" s="9"/>
-      <c r="Y40" s="9"/>
-      <c r="Z40" s="9"/>
+      <c r="Y40" s="11">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="11">
+        <v>1</v>
+      </c>
       <c r="AA40" s="9"/>
     </row>
-    <row r="41" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>135</v>
+    <row r="41" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
@@ -3543,9 +3601,9 @@
       <c r="Z41" s="9"/>
       <c r="AA41" s="9"/>
     </row>
-    <row r="42" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>136</v>
+    <row r="42" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
@@ -3601,9 +3659,9 @@
       <c r="Z42" s="9"/>
       <c r="AA42" s="9"/>
     </row>
-    <row r="43" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>137</v>
+    <row r="43" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="14" t="s">
+        <v>281</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
@@ -3635,9 +3693,9 @@
       <c r="Z43" s="9"/>
       <c r="AA43" s="9"/>
     </row>
-    <row r="44" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>138</v>
+    <row r="44" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
@@ -3669,9 +3727,9 @@
       <c r="Z44" s="9"/>
       <c r="AA44" s="9"/>
     </row>
-    <row r="45" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>139</v>
+    <row r="45" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
@@ -3703,9 +3761,9 @@
       <c r="Z45" s="9"/>
       <c r="AA45" s="9"/>
     </row>
-    <row r="46" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>140</v>
+    <row r="46" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="14" t="s">
+        <v>310</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
@@ -3763,9 +3821,9 @@
       <c r="Z46" s="9"/>
       <c r="AA46" s="9"/>
     </row>
-    <row r="47" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>141</v>
+    <row r="47" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
@@ -3815,9 +3873,9 @@
       <c r="Z47" s="9"/>
       <c r="AA47" s="9"/>
     </row>
-    <row r="48" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>289</v>
+    <row r="48" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="14" t="s">
+        <v>303</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
@@ -3849,9 +3907,9 @@
       <c r="Z48" s="9"/>
       <c r="AA48" s="9"/>
     </row>
-    <row r="49" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>142</v>
+    <row r="49" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
@@ -3901,9 +3959,9 @@
       </c>
       <c r="AA49" s="9"/>
     </row>
-    <row r="50" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>143</v>
+    <row r="50" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
@@ -3935,9 +3993,9 @@
       <c r="Z50" s="9"/>
       <c r="AA50" s="9"/>
     </row>
-    <row r="51" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>144</v>
+    <row r="51" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="14" t="s">
+        <v>139</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
@@ -3993,9 +4051,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>145</v>
+    <row r="52" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="14" t="s">
+        <v>282</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
@@ -4039,9 +4097,9 @@
       <c r="Z52" s="9"/>
       <c r="AA52" s="9"/>
     </row>
-    <row r="53" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>146</v>
+    <row r="53" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="14" t="s">
+        <v>140</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
@@ -4091,9 +4149,9 @@
       </c>
       <c r="AA53" s="9"/>
     </row>
-    <row r="54" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>147</v>
+    <row r="54" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
@@ -4125,9 +4183,9 @@
       <c r="Z54" s="9"/>
       <c r="AA54" s="9"/>
     </row>
-    <row r="55" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>290</v>
+    <row r="55" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
@@ -4183,9 +4241,9 @@
       <c r="Z55" s="9"/>
       <c r="AA55" s="9"/>
     </row>
-    <row r="56" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>148</v>
+    <row r="56" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
@@ -4217,9 +4275,9 @@
       <c r="Z56" s="9"/>
       <c r="AA56" s="9"/>
     </row>
-    <row r="57" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>149</v>
+    <row r="57" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
@@ -4251,9 +4309,9 @@
       <c r="Z57" s="9"/>
       <c r="AA57" s="9"/>
     </row>
-    <row r="58" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>150</v>
+    <row r="58" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="14" t="s">
+        <v>311</v>
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
@@ -4285,9 +4343,9 @@
       <c r="Z58" s="9"/>
       <c r="AA58" s="9"/>
     </row>
-    <row r="59" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>151</v>
+    <row r="59" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="14" t="s">
+        <v>283</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
@@ -4319,9 +4377,9 @@
       <c r="Z59" s="9"/>
       <c r="AA59" s="9"/>
     </row>
-    <row r="60" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>152</v>
+    <row r="60" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
@@ -4367,9 +4425,9 @@
       <c r="Z60" s="9"/>
       <c r="AA60" s="9"/>
     </row>
-    <row r="61" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>153</v>
+    <row r="61" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
@@ -4405,9 +4463,9 @@
       <c r="Z61" s="9"/>
       <c r="AA61" s="9"/>
     </row>
-    <row r="62" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>154</v>
+    <row r="62" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
@@ -4449,9 +4507,9 @@
       </c>
       <c r="AA62" s="9"/>
     </row>
-    <row r="63" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>291</v>
+    <row r="63" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="14" t="s">
+        <v>312</v>
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
@@ -4483,9 +4541,9 @@
       <c r="Z63" s="9"/>
       <c r="AA63" s="9"/>
     </row>
-    <row r="64" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>155</v>
+    <row r="64" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="14" t="s">
+        <v>148</v>
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
@@ -4517,9 +4575,9 @@
       <c r="Z64" s="9"/>
       <c r="AA64" s="9"/>
     </row>
-    <row r="65" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>292</v>
+    <row r="65" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="14" t="s">
+        <v>149</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
@@ -4565,9 +4623,9 @@
       <c r="Z65" s="9"/>
       <c r="AA65" s="9"/>
     </row>
-    <row r="66" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>156</v>
+    <row r="66" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
@@ -4645,9 +4703,9 @@
       </c>
       <c r="AA66" s="9"/>
     </row>
-    <row r="67" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>293</v>
+    <row r="67" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="14" t="s">
+        <v>284</v>
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B130" si="1">SUM(C67:CX67)</f>
@@ -4679,9 +4737,9 @@
       <c r="Z67" s="9"/>
       <c r="AA67" s="9"/>
     </row>
-    <row r="68" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>157</v>
+    <row r="68" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="B68">
         <f t="shared" si="1"/>
@@ -4735,9 +4793,9 @@
       </c>
       <c r="AA68" s="9"/>
     </row>
-    <row r="69" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>158</v>
+    <row r="69" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="14" t="s">
+        <v>285</v>
       </c>
       <c r="B69">
         <f t="shared" si="1"/>
@@ -4787,9 +4845,9 @@
       <c r="Z69" s="9"/>
       <c r="AA69" s="9"/>
     </row>
-    <row r="70" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>159</v>
+    <row r="70" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
@@ -4821,9 +4879,9 @@
       <c r="Z70" s="9"/>
       <c r="AA70" s="9"/>
     </row>
-    <row r="71" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>294</v>
+    <row r="71" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="14" t="s">
+        <v>286</v>
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
@@ -4881,9 +4939,9 @@
       <c r="Z71" s="9"/>
       <c r="AA71" s="9"/>
     </row>
-    <row r="72" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>160</v>
+    <row r="72" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="14" t="s">
+        <v>153</v>
       </c>
       <c r="B72">
         <f t="shared" si="1"/>
@@ -4915,9 +4973,9 @@
       <c r="Z72" s="9"/>
       <c r="AA72" s="9"/>
     </row>
-    <row r="73" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>161</v>
+    <row r="73" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="14" t="s">
+        <v>154</v>
       </c>
       <c r="B73">
         <f t="shared" si="1"/>
@@ -4973,9 +5031,9 @@
       <c r="Z73" s="9"/>
       <c r="AA73" s="9"/>
     </row>
-    <row r="74" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>162</v>
+    <row r="74" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="B74">
         <f t="shared" si="1"/>
@@ -5007,9 +5065,9 @@
       <c r="Z74" s="9"/>
       <c r="AA74" s="9"/>
     </row>
-    <row r="75" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>163</v>
+    <row r="75" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="14" t="s">
+        <v>287</v>
       </c>
       <c r="B75">
         <f t="shared" si="1"/>
@@ -5041,9 +5099,9 @@
       <c r="Z75" s="9"/>
       <c r="AA75" s="9"/>
     </row>
-    <row r="76" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>164</v>
+    <row r="76" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="14" t="s">
+        <v>156</v>
       </c>
       <c r="B76">
         <f t="shared" si="1"/>
@@ -5075,9 +5133,9 @@
       <c r="Z76" s="9"/>
       <c r="AA76" s="9"/>
     </row>
-    <row r="77" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>165</v>
+    <row r="77" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="14" t="s">
+        <v>157</v>
       </c>
       <c r="B77">
         <f t="shared" si="1"/>
@@ -5109,9 +5167,9 @@
       <c r="Z77" s="9"/>
       <c r="AA77" s="9"/>
     </row>
-    <row r="78" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>166</v>
+    <row r="78" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="14" t="s">
+        <v>158</v>
       </c>
       <c r="B78">
         <f t="shared" si="1"/>
@@ -5143,9 +5201,9 @@
       <c r="Z78" s="9"/>
       <c r="AA78" s="9"/>
     </row>
-    <row r="79" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>167</v>
+    <row r="79" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="B79">
         <f t="shared" si="1"/>
@@ -5185,9 +5243,9 @@
       <c r="Z79" s="9"/>
       <c r="AA79" s="9"/>
     </row>
-    <row r="80" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>168</v>
+    <row r="80" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="14" t="s">
+        <v>160</v>
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
@@ -5231,9 +5289,9 @@
       <c r="Z80" s="9"/>
       <c r="AA80" s="9"/>
     </row>
-    <row r="81" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>169</v>
+    <row r="81" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="14" t="s">
+        <v>161</v>
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
@@ -5313,9 +5371,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>170</v>
+    <row r="82" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
@@ -5361,9 +5419,9 @@
       <c r="Z82" s="9"/>
       <c r="AA82" s="9"/>
     </row>
-    <row r="83" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>171</v>
+    <row r="83" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="14" t="s">
+        <v>163</v>
       </c>
       <c r="B83">
         <f t="shared" si="1"/>
@@ -5395,9 +5453,9 @@
       <c r="Z83" s="9"/>
       <c r="AA83" s="9"/>
     </row>
-    <row r="84" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>172</v>
+    <row r="84" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="14" t="s">
+        <v>164</v>
       </c>
       <c r="B84">
         <f t="shared" si="1"/>
@@ -5431,9 +5489,9 @@
       <c r="Z84" s="9"/>
       <c r="AA84" s="9"/>
     </row>
-    <row r="85" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>173</v>
+    <row r="85" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="14" t="s">
+        <v>165</v>
       </c>
       <c r="B85">
         <f t="shared" si="1"/>
@@ -5483,9 +5541,9 @@
       <c r="Z85" s="9"/>
       <c r="AA85" s="9"/>
     </row>
-    <row r="86" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>174</v>
+    <row r="86" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="14" t="s">
+        <v>166</v>
       </c>
       <c r="B86">
         <f t="shared" si="1"/>
@@ -5551,9 +5609,9 @@
       </c>
       <c r="AA86" s="9"/>
     </row>
-    <row r="87" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>175</v>
+    <row r="87" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="14" t="s">
+        <v>167</v>
       </c>
       <c r="B87">
         <f t="shared" si="1"/>
@@ -5585,9 +5643,9 @@
       <c r="Z87" s="9"/>
       <c r="AA87" s="9"/>
     </row>
-    <row r="88" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>176</v>
+    <row r="88" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="B88">
         <f t="shared" si="1"/>
@@ -5619,9 +5677,9 @@
       <c r="Z88" s="9"/>
       <c r="AA88" s="9"/>
     </row>
-    <row r="89" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>295</v>
+    <row r="89" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="B89">
         <f t="shared" si="1"/>
@@ -5653,9 +5711,9 @@
       <c r="Z89" s="9"/>
       <c r="AA89" s="9"/>
     </row>
-    <row r="90" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>177</v>
+    <row r="90" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="B90">
         <f t="shared" si="1"/>
@@ -5687,9 +5745,9 @@
       <c r="Z90" s="9"/>
       <c r="AA90" s="9"/>
     </row>
-    <row r="91" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>178</v>
+    <row r="91" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="B91">
         <f t="shared" si="1"/>
@@ -5745,9 +5803,9 @@
       <c r="Z91" s="9"/>
       <c r="AA91" s="9"/>
     </row>
-    <row r="92" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>179</v>
+    <row r="92" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="14" t="s">
+        <v>172</v>
       </c>
       <c r="B92">
         <f t="shared" si="1"/>
@@ -5779,9 +5837,9 @@
       <c r="Z92" s="9"/>
       <c r="AA92" s="9"/>
     </row>
-    <row r="93" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>296</v>
+    <row r="93" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="14" t="s">
+        <v>288</v>
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
@@ -5817,9 +5875,9 @@
       <c r="Z93" s="9"/>
       <c r="AA93" s="9"/>
     </row>
-    <row r="94" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>180</v>
+    <row r="94" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="B94">
         <f t="shared" si="1"/>
@@ -5851,9 +5909,9 @@
       <c r="Z94" s="9"/>
       <c r="AA94" s="9"/>
     </row>
-    <row r="95" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>181</v>
+    <row r="95" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="14" t="s">
+        <v>174</v>
       </c>
       <c r="B95">
         <f t="shared" si="1"/>
@@ -5897,9 +5955,9 @@
       </c>
       <c r="AA95" s="9"/>
     </row>
-    <row r="96" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>297</v>
+    <row r="96" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="14" t="s">
+        <v>175</v>
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
@@ -5945,9 +6003,9 @@
       <c r="Z96" s="9"/>
       <c r="AA96" s="9"/>
     </row>
-    <row r="97" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>182</v>
+    <row r="97" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="14" t="s">
+        <v>304</v>
       </c>
       <c r="B97">
         <f t="shared" si="1"/>
@@ -5991,9 +6049,9 @@
       <c r="Z97" s="9"/>
       <c r="AA97" s="9"/>
     </row>
-    <row r="98" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>183</v>
+    <row r="98" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="14" t="s">
+        <v>289</v>
       </c>
       <c r="B98">
         <f t="shared" si="1"/>
@@ -6035,9 +6093,9 @@
       <c r="Z98" s="9"/>
       <c r="AA98" s="9"/>
     </row>
-    <row r="99" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>184</v>
+    <row r="99" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="14" t="s">
+        <v>176</v>
       </c>
       <c r="B99">
         <f t="shared" si="1"/>
@@ -6095,9 +6153,9 @@
       </c>
       <c r="AA99" s="9"/>
     </row>
-    <row r="100" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>185</v>
+    <row r="100" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="14" t="s">
+        <v>313</v>
       </c>
       <c r="B100">
         <f t="shared" si="1"/>
@@ -6129,9 +6187,9 @@
       <c r="Z100" s="9"/>
       <c r="AA100" s="9"/>
     </row>
-    <row r="101" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>186</v>
+    <row r="101" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="14" t="s">
+        <v>290</v>
       </c>
       <c r="B101">
         <f t="shared" si="1"/>
@@ -6177,9 +6235,9 @@
       <c r="Z101" s="9"/>
       <c r="AA101" s="9"/>
     </row>
-    <row r="102" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>187</v>
+    <row r="102" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="B102">
         <f t="shared" si="1"/>
@@ -6211,9 +6269,9 @@
       <c r="Z102" s="9"/>
       <c r="AA102" s="9"/>
     </row>
-    <row r="103" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>188</v>
+    <row r="103" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="14" t="s">
+        <v>178</v>
       </c>
       <c r="B103">
         <f t="shared" si="1"/>
@@ -6257,9 +6315,9 @@
       <c r="Z103" s="9"/>
       <c r="AA103" s="9"/>
     </row>
-    <row r="104" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>189</v>
+    <row r="104" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="14" t="s">
+        <v>179</v>
       </c>
       <c r="B104">
         <f t="shared" si="1"/>
@@ -6291,9 +6349,9 @@
       <c r="Z104" s="9"/>
       <c r="AA104" s="9"/>
     </row>
-    <row r="105" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>190</v>
+    <row r="105" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="14" t="s">
+        <v>180</v>
       </c>
       <c r="B105">
         <f t="shared" si="1"/>
@@ -6325,9 +6383,9 @@
       <c r="Z105" s="9"/>
       <c r="AA105" s="9"/>
     </row>
-    <row r="106" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>298</v>
+    <row r="106" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="14" t="s">
+        <v>181</v>
       </c>
       <c r="B106">
         <f t="shared" si="1"/>
@@ -6359,9 +6417,9 @@
       <c r="Z106" s="9"/>
       <c r="AA106" s="9"/>
     </row>
-    <row r="107" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>191</v>
+    <row r="107" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="14" t="s">
+        <v>182</v>
       </c>
       <c r="B107">
         <f t="shared" si="1"/>
@@ -6395,9 +6453,9 @@
       <c r="Z107" s="9"/>
       <c r="AA107" s="9"/>
     </row>
-    <row r="108" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>192</v>
+    <row r="108" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="14" t="s">
+        <v>183</v>
       </c>
       <c r="B108">
         <f t="shared" si="1"/>
@@ -6435,9 +6493,9 @@
       <c r="Z108" s="9"/>
       <c r="AA108" s="9"/>
     </row>
-    <row r="109" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>193</v>
+    <row r="109" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="B109">
         <f t="shared" si="1"/>
@@ -6489,9 +6547,9 @@
       <c r="Z109" s="9"/>
       <c r="AA109" s="9"/>
     </row>
-    <row r="110" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>299</v>
+    <row r="110" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="B110">
         <f t="shared" si="1"/>
@@ -6537,9 +6595,9 @@
       <c r="Z110" s="9"/>
       <c r="AA110" s="9"/>
     </row>
-    <row r="111" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>194</v>
+    <row r="111" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="14" t="s">
+        <v>291</v>
       </c>
       <c r="B111">
         <f t="shared" si="1"/>
@@ -6571,9 +6629,9 @@
       <c r="Z111" s="9"/>
       <c r="AA111" s="9"/>
     </row>
-    <row r="112" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>195</v>
+    <row r="112" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="14" t="s">
+        <v>186</v>
       </c>
       <c r="B112">
         <f t="shared" si="1"/>
@@ -6619,9 +6677,9 @@
       <c r="Z112" s="9"/>
       <c r="AA112" s="9"/>
     </row>
-    <row r="113" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>196</v>
+    <row r="113" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="B113">
         <f t="shared" si="1"/>
@@ -6653,9 +6711,9 @@
       <c r="Z113" s="9"/>
       <c r="AA113" s="9"/>
     </row>
-    <row r="114" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>197</v>
+    <row r="114" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="B114">
         <f t="shared" si="1"/>
@@ -6697,9 +6755,9 @@
       <c r="Z114" s="9"/>
       <c r="AA114" s="9"/>
     </row>
-    <row r="115" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>198</v>
+    <row r="115" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="B115">
         <f t="shared" si="1"/>
@@ -6731,9 +6789,9 @@
       <c r="Z115" s="9"/>
       <c r="AA115" s="9"/>
     </row>
-    <row r="116" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>199</v>
+    <row r="116" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="14" t="s">
+        <v>292</v>
       </c>
       <c r="B116">
         <f t="shared" si="1"/>
@@ -6781,9 +6839,9 @@
       <c r="Z116" s="9"/>
       <c r="AA116" s="9"/>
     </row>
-    <row r="117" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>200</v>
+    <row r="117" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="14" t="s">
+        <v>189</v>
       </c>
       <c r="B117">
         <f t="shared" si="1"/>
@@ -6815,9 +6873,9 @@
       <c r="Z117" s="9"/>
       <c r="AA117" s="9"/>
     </row>
-    <row r="118" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>201</v>
+    <row r="118" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="B118">
         <f t="shared" si="1"/>
@@ -6855,9 +6913,9 @@
       <c r="Z118" s="9"/>
       <c r="AA118" s="9"/>
     </row>
-    <row r="119" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>202</v>
+    <row r="119" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="14" t="s">
+        <v>191</v>
       </c>
       <c r="B119">
         <f t="shared" si="1"/>
@@ -6889,9 +6947,9 @@
       <c r="Z119" s="9"/>
       <c r="AA119" s="9"/>
     </row>
-    <row r="120" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>203</v>
+    <row r="120" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="14" t="s">
+        <v>192</v>
       </c>
       <c r="B120">
         <f t="shared" si="1"/>
@@ -6939,9 +6997,9 @@
       <c r="Z120" s="9"/>
       <c r="AA120" s="9"/>
     </row>
-    <row r="121" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>204</v>
+    <row r="121" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="14" t="s">
+        <v>193</v>
       </c>
       <c r="B121">
         <f t="shared" si="1"/>
@@ -6989,9 +7047,9 @@
       <c r="Z121" s="9"/>
       <c r="AA121" s="9"/>
     </row>
-    <row r="122" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>300</v>
+    <row r="122" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="B122">
         <f t="shared" si="1"/>
@@ -7023,9 +7081,9 @@
       <c r="Z122" s="9"/>
       <c r="AA122" s="9"/>
     </row>
-    <row r="123" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>205</v>
+    <row r="123" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A123" s="14" t="s">
+        <v>195</v>
       </c>
       <c r="B123">
         <f t="shared" si="1"/>
@@ -7091,9 +7149,9 @@
       </c>
       <c r="AA123" s="9"/>
     </row>
-    <row r="124" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>206</v>
+    <row r="124" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="14" t="s">
+        <v>196</v>
       </c>
       <c r="B124">
         <f t="shared" si="1"/>
@@ -7131,9 +7189,9 @@
       <c r="Z124" s="9"/>
       <c r="AA124" s="9"/>
     </row>
-    <row r="125" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>207</v>
+    <row r="125" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A125" s="14" t="s">
+        <v>314</v>
       </c>
       <c r="B125">
         <f t="shared" si="1"/>
@@ -7189,9 +7247,9 @@
       <c r="Z125" s="9"/>
       <c r="AA125" s="9"/>
     </row>
-    <row r="126" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>208</v>
+    <row r="126" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A126" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="B126">
         <f t="shared" si="1"/>
@@ -7249,9 +7307,9 @@
       <c r="Z126" s="9"/>
       <c r="AA126" s="9"/>
     </row>
-    <row r="127" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>209</v>
+    <row r="127" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A127" s="14" t="s">
+        <v>198</v>
       </c>
       <c r="B127">
         <f t="shared" si="1"/>
@@ -7305,9 +7363,9 @@
       <c r="Z127" s="9"/>
       <c r="AA127" s="9"/>
     </row>
-    <row r="128" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>210</v>
+    <row r="128" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A128" s="14" t="s">
+        <v>199</v>
       </c>
       <c r="B128">
         <f t="shared" si="1"/>
@@ -7339,9 +7397,9 @@
       <c r="Z128" s="9"/>
       <c r="AA128" s="9"/>
     </row>
-    <row r="129" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>211</v>
+    <row r="129" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A129" s="14" t="s">
+        <v>293</v>
       </c>
       <c r="B129">
         <f t="shared" si="1"/>
@@ -7393,9 +7451,9 @@
       <c r="Z129" s="9"/>
       <c r="AA129" s="9"/>
     </row>
-    <row r="130" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>212</v>
+    <row r="130" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A130" s="14" t="s">
+        <v>306</v>
       </c>
       <c r="B130">
         <f t="shared" si="1"/>
@@ -7439,9 +7497,9 @@
       </c>
       <c r="AA130" s="9"/>
     </row>
-    <row r="131" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>213</v>
+    <row r="131" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A131" s="14" t="s">
+        <v>200</v>
       </c>
       <c r="B131">
         <f t="shared" ref="B131:B194" si="2">SUM(C131:CX131)</f>
@@ -7499,9 +7557,9 @@
       <c r="Z131" s="9"/>
       <c r="AA131" s="9"/>
     </row>
-    <row r="132" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>214</v>
+    <row r="132" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A132" s="14" t="s">
+        <v>201</v>
       </c>
       <c r="B132">
         <f t="shared" si="2"/>
@@ -7577,9 +7635,9 @@
       </c>
       <c r="AA132" s="9"/>
     </row>
-    <row r="133" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>215</v>
+    <row r="133" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A133" s="14" t="s">
+        <v>202</v>
       </c>
       <c r="B133">
         <f t="shared" si="2"/>
@@ -7611,9 +7669,9 @@
       <c r="Z133" s="9"/>
       <c r="AA133" s="9"/>
     </row>
-    <row r="134" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>216</v>
+    <row r="134" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A134" s="14" t="s">
+        <v>203</v>
       </c>
       <c r="B134">
         <f t="shared" si="2"/>
@@ -7657,9 +7715,9 @@
       <c r="Z134" s="9"/>
       <c r="AA134" s="9"/>
     </row>
-    <row r="135" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>217</v>
+    <row r="135" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A135" s="14" t="s">
+        <v>204</v>
       </c>
       <c r="B135">
         <f t="shared" si="2"/>
@@ -7709,9 +7767,9 @@
       <c r="Z135" s="9"/>
       <c r="AA135" s="9"/>
     </row>
-    <row r="136" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>218</v>
+    <row r="136" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A136" s="14" t="s">
+        <v>205</v>
       </c>
       <c r="B136">
         <f t="shared" si="2"/>
@@ -7743,9 +7801,9 @@
       <c r="Z136" s="9"/>
       <c r="AA136" s="9"/>
     </row>
-    <row r="137" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>219</v>
+    <row r="137" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A137" s="14" t="s">
+        <v>206</v>
       </c>
       <c r="B137">
         <f t="shared" si="2"/>
@@ -7777,9 +7835,9 @@
       <c r="Z137" s="9"/>
       <c r="AA137" s="9"/>
     </row>
-    <row r="138" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>220</v>
+    <row r="138" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A138" s="14" t="s">
+        <v>207</v>
       </c>
       <c r="B138">
         <f t="shared" si="2"/>
@@ -7821,9 +7879,9 @@
       </c>
       <c r="AA138" s="9"/>
     </row>
-    <row r="139" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>221</v>
+    <row r="139" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A139" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="B139">
         <f t="shared" si="2"/>
@@ -7881,9 +7939,9 @@
       <c r="Z139" s="9"/>
       <c r="AA139" s="9"/>
     </row>
-    <row r="140" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>301</v>
+    <row r="140" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A140" s="14" t="s">
+        <v>315</v>
       </c>
       <c r="B140">
         <f t="shared" si="2"/>
@@ -7937,9 +7995,9 @@
       <c r="Z140" s="9"/>
       <c r="AA140" s="9"/>
     </row>
-    <row r="141" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>302</v>
+    <row r="141" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A141" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="B141">
         <f t="shared" si="2"/>
@@ -7989,9 +8047,9 @@
       </c>
       <c r="AA141" s="9"/>
     </row>
-    <row r="142" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>222</v>
+    <row r="142" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A142" s="14" t="s">
+        <v>209</v>
       </c>
       <c r="B142">
         <f t="shared" si="2"/>
@@ -8037,9 +8095,9 @@
       <c r="Z142" s="9"/>
       <c r="AA142" s="9"/>
     </row>
-    <row r="143" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>223</v>
+    <row r="143" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A143" s="14" t="s">
+        <v>210</v>
       </c>
       <c r="B143">
         <f t="shared" si="2"/>
@@ -8093,9 +8151,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>224</v>
+    <row r="144" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A144" s="14" t="s">
+        <v>211</v>
       </c>
       <c r="B144">
         <f t="shared" si="2"/>
@@ -8147,9 +8205,9 @@
       </c>
       <c r="AA144" s="9"/>
     </row>
-    <row r="145" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>225</v>
+    <row r="145" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A145" s="14" t="s">
+        <v>212</v>
       </c>
       <c r="B145">
         <f t="shared" si="2"/>
@@ -8203,9 +8261,9 @@
       <c r="Z145" s="9"/>
       <c r="AA145" s="9"/>
     </row>
-    <row r="146" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>226</v>
+    <row r="146" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A146" s="14" t="s">
+        <v>213</v>
       </c>
       <c r="B146">
         <f t="shared" si="2"/>
@@ -8257,9 +8315,9 @@
       <c r="Z146" s="9"/>
       <c r="AA146" s="9"/>
     </row>
-    <row r="147" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>227</v>
+    <row r="147" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A147" s="14" t="s">
+        <v>214</v>
       </c>
       <c r="B147">
         <f t="shared" si="2"/>
@@ -8291,9 +8349,9 @@
       <c r="Z147" s="9"/>
       <c r="AA147" s="9"/>
     </row>
-    <row r="148" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>228</v>
+    <row r="148" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A148" s="14" t="s">
+        <v>215</v>
       </c>
       <c r="B148">
         <f t="shared" si="2"/>
@@ -8325,9 +8383,9 @@
       <c r="Z148" s="9"/>
       <c r="AA148" s="9"/>
     </row>
-    <row r="149" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>229</v>
+    <row r="149" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A149" s="14" t="s">
+        <v>294</v>
       </c>
       <c r="B149">
         <f t="shared" si="2"/>
@@ -8381,9 +8439,9 @@
       <c r="Z149" s="9"/>
       <c r="AA149" s="9"/>
     </row>
-    <row r="150" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>230</v>
+    <row r="150" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A150" s="14" t="s">
+        <v>295</v>
       </c>
       <c r="B150">
         <f t="shared" si="2"/>
@@ -8415,9 +8473,9 @@
       <c r="Z150" s="9"/>
       <c r="AA150" s="9"/>
     </row>
-    <row r="151" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>303</v>
+    <row r="151" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A151" s="14" t="s">
+        <v>216</v>
       </c>
       <c r="B151">
         <f t="shared" si="2"/>
@@ -8449,9 +8507,9 @@
       <c r="Z151" s="9"/>
       <c r="AA151" s="9"/>
     </row>
-    <row r="152" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>231</v>
+    <row r="152" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A152" s="14" t="s">
+        <v>217</v>
       </c>
       <c r="B152">
         <f t="shared" si="2"/>
@@ -8489,9 +8547,9 @@
       </c>
       <c r="AA152" s="9"/>
     </row>
-    <row r="153" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>232</v>
+    <row r="153" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A153" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="B153">
         <f t="shared" si="2"/>
@@ -8537,9 +8595,9 @@
       <c r="Z153" s="9"/>
       <c r="AA153" s="9"/>
     </row>
-    <row r="154" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>233</v>
+    <row r="154" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A154" s="14" t="s">
+        <v>316</v>
       </c>
       <c r="B154">
         <f t="shared" si="2"/>
@@ -8593,9 +8651,9 @@
       </c>
       <c r="AA154" s="9"/>
     </row>
-    <row r="155" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>234</v>
+    <row r="155" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="14" t="s">
+        <v>219</v>
       </c>
       <c r="B155">
         <f t="shared" si="2"/>
@@ -8639,9 +8697,9 @@
       <c r="Z155" s="9"/>
       <c r="AA155" s="9"/>
     </row>
-    <row r="156" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>235</v>
+    <row r="156" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A156" s="14" t="s">
+        <v>220</v>
       </c>
       <c r="B156">
         <f t="shared" si="2"/>
@@ -8697,9 +8755,9 @@
       </c>
       <c r="AA156" s="9"/>
     </row>
-    <row r="157" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
-        <v>236</v>
+    <row r="157" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A157" s="14" t="s">
+        <v>221</v>
       </c>
       <c r="B157">
         <f t="shared" si="2"/>
@@ -8741,9 +8799,9 @@
       </c>
       <c r="AA157" s="9"/>
     </row>
-    <row r="158" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>237</v>
+    <row r="158" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A158" s="14" t="s">
+        <v>222</v>
       </c>
       <c r="B158">
         <f t="shared" si="2"/>
@@ -8795,9 +8853,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>304</v>
+    <row r="159" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A159" s="14" t="s">
+        <v>223</v>
       </c>
       <c r="B159">
         <f t="shared" si="2"/>
@@ -8829,9 +8887,9 @@
       <c r="Z159" s="9"/>
       <c r="AA159" s="9"/>
     </row>
-    <row r="160" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>238</v>
+    <row r="160" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A160" s="14" t="s">
+        <v>224</v>
       </c>
       <c r="B160">
         <f t="shared" si="2"/>
@@ -8883,9 +8941,9 @@
       <c r="Z160" s="9"/>
       <c r="AA160" s="9"/>
     </row>
-    <row r="161" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>239</v>
+    <row r="161" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A161" s="14" t="s">
+        <v>296</v>
       </c>
       <c r="B161">
         <f t="shared" si="2"/>
@@ -8923,9 +8981,9 @@
       <c r="Z161" s="9"/>
       <c r="AA161" s="9"/>
     </row>
-    <row r="162" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>240</v>
+    <row r="162" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A162" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="B162">
         <f t="shared" si="2"/>
@@ -8977,9 +9035,9 @@
       <c r="Z162" s="9"/>
       <c r="AA162" s="9"/>
     </row>
-    <row r="163" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>241</v>
+    <row r="163" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A163" s="14" t="s">
+        <v>226</v>
       </c>
       <c r="B163">
         <f t="shared" si="2"/>
@@ -9025,9 +9083,9 @@
       <c r="Z163" s="9"/>
       <c r="AA163" s="9"/>
     </row>
-    <row r="164" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
-        <v>242</v>
+    <row r="164" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A164" s="14" t="s">
+        <v>227</v>
       </c>
       <c r="B164">
         <f t="shared" si="2"/>
@@ -9059,9 +9117,9 @@
       <c r="Z164" s="9"/>
       <c r="AA164" s="9"/>
     </row>
-    <row r="165" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
-        <v>243</v>
+    <row r="165" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A165" s="14" t="s">
+        <v>228</v>
       </c>
       <c r="B165">
         <f t="shared" si="2"/>
@@ -9093,9 +9151,9 @@
       <c r="Z165" s="9"/>
       <c r="AA165" s="9"/>
     </row>
-    <row r="166" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
-        <v>244</v>
+    <row r="166" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A166" s="14" t="s">
+        <v>229</v>
       </c>
       <c r="B166">
         <f t="shared" si="2"/>
@@ -9127,9 +9185,9 @@
       <c r="Z166" s="9"/>
       <c r="AA166" s="9"/>
     </row>
-    <row r="167" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
-        <v>245</v>
+    <row r="167" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A167" s="14" t="s">
+        <v>230</v>
       </c>
       <c r="B167">
         <f t="shared" si="2"/>
@@ -9167,9 +9225,9 @@
       <c r="Z167" s="9"/>
       <c r="AA167" s="9"/>
     </row>
-    <row r="168" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
-        <v>246</v>
+    <row r="168" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A168" s="14" t="s">
+        <v>231</v>
       </c>
       <c r="B168">
         <f t="shared" si="2"/>
@@ -9201,9 +9259,9 @@
       <c r="Z168" s="9"/>
       <c r="AA168" s="9"/>
     </row>
-    <row r="169" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
-        <v>247</v>
+    <row r="169" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A169" s="14" t="s">
+        <v>297</v>
       </c>
       <c r="B169">
         <f t="shared" si="2"/>
@@ -9239,9 +9297,9 @@
       <c r="Z169" s="9"/>
       <c r="AA169" s="9"/>
     </row>
-    <row r="170" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
-        <v>248</v>
+    <row r="170" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A170" s="14" t="s">
+        <v>232</v>
       </c>
       <c r="B170">
         <f t="shared" si="2"/>
@@ -9273,9 +9331,9 @@
       <c r="Z170" s="9"/>
       <c r="AA170" s="9"/>
     </row>
-    <row r="171" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
-        <v>249</v>
+    <row r="171" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A171" s="14" t="s">
+        <v>233</v>
       </c>
       <c r="B171">
         <f t="shared" si="2"/>
@@ -9307,9 +9365,9 @@
       <c r="Z171" s="9"/>
       <c r="AA171" s="9"/>
     </row>
-    <row r="172" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
-        <v>250</v>
+    <row r="172" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A172" s="14" t="s">
+        <v>234</v>
       </c>
       <c r="B172">
         <f t="shared" si="2"/>
@@ -9341,9 +9399,9 @@
       <c r="Z172" s="9"/>
       <c r="AA172" s="9"/>
     </row>
-    <row r="173" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
-        <v>251</v>
+    <row r="173" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A173" s="14" t="s">
+        <v>235</v>
       </c>
       <c r="B173">
         <f t="shared" si="2"/>
@@ -9393,9 +9451,9 @@
       <c r="Z173" s="9"/>
       <c r="AA173" s="9"/>
     </row>
-    <row r="174" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
-        <v>252</v>
+    <row r="174" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A174" s="14" t="s">
+        <v>236</v>
       </c>
       <c r="B174">
         <f t="shared" si="2"/>
@@ -9427,9 +9485,9 @@
       <c r="Z174" s="9"/>
       <c r="AA174" s="9"/>
     </row>
-    <row r="175" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
-        <v>253</v>
+    <row r="175" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A175" s="14" t="s">
+        <v>237</v>
       </c>
       <c r="B175">
         <f t="shared" si="2"/>
@@ -9461,9 +9519,9 @@
       <c r="Z175" s="9"/>
       <c r="AA175" s="9"/>
     </row>
-    <row r="176" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
-        <v>254</v>
+    <row r="176" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A176" s="14" t="s">
+        <v>238</v>
       </c>
       <c r="B176">
         <f t="shared" si="2"/>
@@ -9513,9 +9571,9 @@
       <c r="Z176" s="9"/>
       <c r="AA176" s="9"/>
     </row>
-    <row r="177" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
-        <v>255</v>
+    <row r="177" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A177" s="14" t="s">
+        <v>239</v>
       </c>
       <c r="B177">
         <f t="shared" si="2"/>
@@ -9561,9 +9619,9 @@
       <c r="Z177" s="9"/>
       <c r="AA177" s="9"/>
     </row>
-    <row r="178" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
-        <v>256</v>
+    <row r="178" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A178" s="14" t="s">
+        <v>240</v>
       </c>
       <c r="B178">
         <f t="shared" si="2"/>
@@ -9611,9 +9669,9 @@
       <c r="Z178" s="9"/>
       <c r="AA178" s="9"/>
     </row>
-    <row r="179" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
-        <v>257</v>
+    <row r="179" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A179" s="14" t="s">
+        <v>241</v>
       </c>
       <c r="B179">
         <f t="shared" si="2"/>
@@ -9659,9 +9717,9 @@
       <c r="Z179" s="9"/>
       <c r="AA179" s="9"/>
     </row>
-    <row r="180" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
-        <v>305</v>
+    <row r="180" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A180" s="14" t="s">
+        <v>317</v>
       </c>
       <c r="B180">
         <f t="shared" si="2"/>
@@ -9703,9 +9761,9 @@
       <c r="Z180" s="9"/>
       <c r="AA180" s="9"/>
     </row>
-    <row r="181" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" t="s">
-        <v>258</v>
+    <row r="181" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A181" s="14" t="s">
+        <v>242</v>
       </c>
       <c r="B181">
         <f t="shared" si="2"/>
@@ -9737,9 +9795,9 @@
       <c r="Z181" s="9"/>
       <c r="AA181" s="9"/>
     </row>
-    <row r="182" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
-        <v>259</v>
+    <row r="182" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A182" s="14" t="s">
+        <v>243</v>
       </c>
       <c r="B182">
         <f t="shared" si="2"/>
@@ -9771,9 +9829,9 @@
       <c r="Z182" s="9"/>
       <c r="AA182" s="9"/>
     </row>
-    <row r="183" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
-        <v>260</v>
+    <row r="183" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A183" s="14" t="s">
+        <v>244</v>
       </c>
       <c r="B183">
         <f t="shared" si="2"/>
@@ -9805,9 +9863,9 @@
       <c r="Z183" s="9"/>
       <c r="AA183" s="9"/>
     </row>
-    <row r="184" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
-        <v>261</v>
+    <row r="184" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A184" s="14" t="s">
+        <v>245</v>
       </c>
       <c r="B184">
         <f t="shared" si="2"/>
@@ -9839,9 +9897,9 @@
       <c r="Z184" s="9"/>
       <c r="AA184" s="9"/>
     </row>
-    <row r="185" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" t="s">
-        <v>262</v>
+    <row r="185" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A185" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="B185">
         <f t="shared" si="2"/>
@@ -9887,9 +9945,9 @@
       <c r="Z185" s="9"/>
       <c r="AA185" s="9"/>
     </row>
-    <row r="186" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
-        <v>263</v>
+    <row r="186" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A186" s="14" t="s">
+        <v>247</v>
       </c>
       <c r="B186">
         <f t="shared" si="2"/>
@@ -9921,9 +9979,9 @@
       <c r="Z186" s="9"/>
       <c r="AA186" s="9"/>
     </row>
-    <row r="187" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
-        <v>264</v>
+    <row r="187" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A187" s="14" t="s">
+        <v>248</v>
       </c>
       <c r="B187">
         <f t="shared" si="2"/>
@@ -9955,9 +10013,9 @@
       <c r="Z187" s="9"/>
       <c r="AA187" s="9"/>
     </row>
-    <row r="188" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
-        <v>265</v>
+    <row r="188" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A188" s="14" t="s">
+        <v>249</v>
       </c>
       <c r="B188">
         <f t="shared" si="2"/>
@@ -9989,9 +10047,9 @@
       <c r="Z188" s="9"/>
       <c r="AA188" s="9"/>
     </row>
-    <row r="189" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
-        <v>266</v>
+    <row r="189" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A189" s="14" t="s">
+        <v>250</v>
       </c>
       <c r="B189">
         <f t="shared" si="2"/>
@@ -10023,9 +10081,9 @@
       <c r="Z189" s="9"/>
       <c r="AA189" s="9"/>
     </row>
-    <row r="190" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
-        <v>267</v>
+    <row r="190" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A190" s="14" t="s">
+        <v>298</v>
       </c>
       <c r="B190">
         <f t="shared" si="2"/>
@@ -10065,9 +10123,9 @@
       <c r="Z190" s="9"/>
       <c r="AA190" s="9"/>
     </row>
-    <row r="191" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
-        <v>268</v>
+    <row r="191" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A191" s="14" t="s">
+        <v>251</v>
       </c>
       <c r="B191">
         <f t="shared" si="2"/>
@@ -10119,9 +10177,9 @@
       <c r="Z191" s="9"/>
       <c r="AA191" s="9"/>
     </row>
-    <row r="192" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A192" t="s">
-        <v>269</v>
+    <row r="192" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A192" s="14" t="s">
+        <v>252</v>
       </c>
       <c r="B192">
         <f t="shared" si="2"/>
@@ -10153,9 +10211,9 @@
       <c r="Z192" s="9"/>
       <c r="AA192" s="9"/>
     </row>
-    <row r="193" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
-        <v>270</v>
+    <row r="193" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A193" s="14" t="s">
+        <v>253</v>
       </c>
       <c r="B193">
         <f t="shared" si="2"/>
@@ -10187,9 +10245,9 @@
       <c r="Z193" s="9"/>
       <c r="AA193" s="9"/>
     </row>
-    <row r="194" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" t="s">
-        <v>271</v>
+    <row r="194" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A194" s="14" t="s">
+        <v>254</v>
       </c>
       <c r="B194">
         <f t="shared" si="2"/>
@@ -10221,12 +10279,12 @@
       <c r="Z194" s="9"/>
       <c r="AA194" s="9"/>
     </row>
-    <row r="195" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
-        <v>272</v>
+    <row r="195" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A195" s="14" t="s">
+        <v>255</v>
       </c>
       <c r="B195">
-        <f t="shared" ref="B195:B207" si="3">SUM(C195:CX195)</f>
+        <f t="shared" ref="B195:B217" si="3">SUM(C195:CX195)</f>
         <v>11</v>
       </c>
       <c r="C195" s="6">
@@ -10277,9 +10335,9 @@
       <c r="Z195" s="9"/>
       <c r="AA195" s="9"/>
     </row>
-    <row r="196" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
-        <v>273</v>
+    <row r="196" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A196" s="14" t="s">
+        <v>256</v>
       </c>
       <c r="B196">
         <f t="shared" si="3"/>
@@ -10329,9 +10387,9 @@
       <c r="Z196" s="9"/>
       <c r="AA196" s="9"/>
     </row>
-    <row r="197" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
-        <v>274</v>
+    <row r="197" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A197" s="14" t="s">
+        <v>257</v>
       </c>
       <c r="B197">
         <f t="shared" si="3"/>
@@ -10363,9 +10421,9 @@
       <c r="Z197" s="9"/>
       <c r="AA197" s="9"/>
     </row>
-    <row r="198" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
-        <v>306</v>
+    <row r="198" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A198" s="14" t="s">
+        <v>258</v>
       </c>
       <c r="B198">
         <f t="shared" si="3"/>
@@ -10413,9 +10471,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
-        <v>275</v>
+    <row r="199" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A199" s="14" t="s">
+        <v>259</v>
       </c>
       <c r="B199">
         <f t="shared" si="3"/>
@@ -10469,9 +10527,9 @@
       <c r="Z199" s="9"/>
       <c r="AA199" s="9"/>
     </row>
-    <row r="200" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
-        <v>276</v>
+    <row r="200" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A200" s="14" t="s">
+        <v>260</v>
       </c>
       <c r="B200">
         <f t="shared" si="3"/>
@@ -10519,9 +10577,9 @@
       <c r="Z200" s="9"/>
       <c r="AA200" s="9"/>
     </row>
-    <row r="201" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
-        <v>277</v>
+    <row r="201" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A201" s="14" t="s">
+        <v>261</v>
       </c>
       <c r="B201">
         <f t="shared" si="3"/>
@@ -10553,9 +10611,9 @@
       <c r="Z201" s="9"/>
       <c r="AA201" s="9"/>
     </row>
-    <row r="202" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
-        <v>278</v>
+    <row r="202" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A202" s="14" t="s">
+        <v>262</v>
       </c>
       <c r="B202">
         <f t="shared" si="3"/>
@@ -10593,9 +10651,9 @@
       <c r="Z202" s="9"/>
       <c r="AA202" s="9"/>
     </row>
-    <row r="203" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" t="s">
-        <v>279</v>
+    <row r="203" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A203" s="14" t="s">
+        <v>263</v>
       </c>
       <c r="B203">
         <f t="shared" si="3"/>
@@ -10639,9 +10697,9 @@
       <c r="Z203" s="9"/>
       <c r="AA203" s="9"/>
     </row>
-    <row r="204" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
-        <v>280</v>
+    <row r="204" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A204" s="14" t="s">
+        <v>264</v>
       </c>
       <c r="B204">
         <f t="shared" si="3"/>
@@ -10717,9 +10775,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205" t="s">
-        <v>281</v>
+    <row r="205" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A205" s="14" t="s">
+        <v>265</v>
       </c>
       <c r="B205">
         <f t="shared" si="3"/>
@@ -10801,9 +10859,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
-        <v>307</v>
+    <row r="206" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A206" s="14" t="s">
+        <v>266</v>
       </c>
       <c r="B206">
         <f t="shared" si="3"/>
@@ -10857,9 +10915,9 @@
       </c>
       <c r="AA206" s="9"/>
     </row>
-    <row r="207" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A207" t="s">
-        <v>282</v>
+    <row r="207" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A207" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="B207">
         <f t="shared" si="3"/>
@@ -10891,7 +10949,14 @@
       <c r="Z207" s="9"/>
       <c r="AA207" s="9"/>
     </row>
-    <row r="208" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A208" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="B208">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
       <c r="C208" s="10"/>
       <c r="D208" s="8"/>
       <c r="E208" s="8"/>
@@ -10938,7 +11003,14 @@
       </c>
       <c r="AA208" s="9"/>
     </row>
-    <row r="209" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A209" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B209">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
       <c r="C209" s="10"/>
       <c r="D209" s="8"/>
       <c r="E209" s="8"/>
@@ -10983,7 +11055,14 @@
       </c>
       <c r="AA209" s="9"/>
     </row>
-    <row r="210" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A210" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B210">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="C210" s="10"/>
       <c r="D210" s="8"/>
       <c r="E210" s="8"/>
@@ -11010,7 +11089,14 @@
       <c r="Z210" s="9"/>
       <c r="AA210" s="9"/>
     </row>
-    <row r="211" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A211" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B211">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
       <c r="C211" s="6">
         <v>1</v>
       </c>
@@ -11087,7 +11173,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A212" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="B212">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
       <c r="C212" s="6">
         <v>1</v>
       </c>
@@ -11156,7 +11249,14 @@
       </c>
       <c r="AA212" s="9"/>
     </row>
-    <row r="213" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A213" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="B213">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
       <c r="C213" s="6">
         <v>1</v>
       </c>
@@ -11205,7 +11305,14 @@
       </c>
       <c r="AA213" s="9"/>
     </row>
-    <row r="214" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A214" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B214">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
       <c r="C214" s="6">
         <v>1</v>
       </c>
@@ -11254,7 +11361,14 @@
       <c r="Z214" s="9"/>
       <c r="AA214" s="9"/>
     </row>
-    <row r="215" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A215" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="B215">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
       <c r="C215" s="10"/>
       <c r="D215" s="8"/>
       <c r="E215" s="8"/>
@@ -11293,7 +11407,14 @@
       </c>
       <c r="AA215" s="9"/>
     </row>
-    <row r="216" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A216" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B216">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="C216" s="10"/>
       <c r="D216" s="8"/>
       <c r="E216" s="8"/>
@@ -11320,7 +11441,14 @@
       <c r="Z216" s="9"/>
       <c r="AA216" s="9"/>
     </row>
-    <row r="217" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A217" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="B217">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="C217" s="10"/>
       <c r="D217" s="8"/>
       <c r="E217" s="8"/>
@@ -11349,5 +11477,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20251013 - Score updates
</commit_message>
<xml_diff>
--- a/assets/score/bxb-template.xlsx
+++ b/assets/score/bxb-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PWRCh\OneDrive\Desktop\gitproject\bxbscore\assets\score\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1848F7-BBC7-4C2A-98F4-7B7425D32A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F607BF53-E057-4918-9307-DA0D05FF5ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{7F520E0E-A91E-45B5-A85D-62EFB1C3D427}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AA196" authorId="0" shapeId="0" xr:uid="{E42C26AB-1423-4BFC-9CB0-103777AF6897}">
+    <comment ref="AA196" authorId="0" shapeId="0" xr:uid="{DAC82235-DE85-442D-AB5D-BAE5885C745A}">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="345">
   <si>
     <t>Participant Name</t>
   </si>
@@ -1094,6 +1094,9 @@
   <si>
     <t>Tan Cheng Tat</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -2508,7 +2511,7 @@
       </c>
       <c r="B5" s="11">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
@@ -2631,17 +2634,33 @@
         <v>1</v>
       </c>
       <c r="BA5" s="17"/>
-      <c r="BB5" s="3"/>
-      <c r="BC5" s="3"/>
+      <c r="BB5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC5" s="3">
+        <v>1</v>
+      </c>
       <c r="BD5" s="3"/>
-      <c r="BE5" s="3"/>
-      <c r="BF5" s="3"/>
+      <c r="BE5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF5" s="3">
+        <v>1</v>
+      </c>
       <c r="BG5" s="3"/>
-      <c r="BH5" s="3"/>
+      <c r="BH5" s="3">
+        <v>1</v>
+      </c>
       <c r="BI5" s="3"/>
-      <c r="BJ5" s="3"/>
-      <c r="BK5" s="3"/>
-      <c r="BL5" s="3"/>
+      <c r="BJ5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL5" s="3">
+        <v>1</v>
+      </c>
       <c r="BM5" s="4"/>
       <c r="BN5" s="4"/>
       <c r="BO5" s="4">
@@ -2852,7 +2871,7 @@
       </c>
       <c r="B7" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="3"/>
@@ -2944,19 +2963,33 @@
       <c r="BJ7" s="3"/>
       <c r="BK7" s="3"/>
       <c r="BL7" s="3"/>
-      <c r="BM7" s="4"/>
+      <c r="BM7" s="4">
+        <v>1</v>
+      </c>
       <c r="BN7" s="4"/>
-      <c r="BO7" s="4"/>
-      <c r="BP7" s="4"/>
+      <c r="BO7" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP7" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ7" s="4"/>
       <c r="BR7" s="4"/>
       <c r="BS7" s="4"/>
       <c r="BT7" s="4"/>
-      <c r="BU7" s="4"/>
+      <c r="BU7" s="4">
+        <v>1</v>
+      </c>
       <c r="BV7" s="4"/>
-      <c r="BW7" s="4"/>
-      <c r="BX7" s="4"/>
-      <c r="BY7" s="18"/>
+      <c r="BW7" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX7" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY7" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:102" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
@@ -3196,7 +3229,7 @@
       </c>
       <c r="B9" s="11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="3"/>
@@ -3275,17 +3308,29 @@
         <v>1</v>
       </c>
       <c r="BA9" s="17"/>
-      <c r="BB9" s="3"/>
+      <c r="BB9" s="3">
+        <v>1</v>
+      </c>
       <c r="BC9" s="3"/>
       <c r="BD9" s="3"/>
-      <c r="BE9" s="3"/>
-      <c r="BF9" s="3"/>
+      <c r="BE9" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF9" s="3">
+        <v>1</v>
+      </c>
       <c r="BG9" s="3"/>
-      <c r="BH9" s="3"/>
+      <c r="BH9" s="3">
+        <v>1</v>
+      </c>
       <c r="BI9" s="3"/>
-      <c r="BJ9" s="3"/>
+      <c r="BJ9" s="3">
+        <v>1</v>
+      </c>
       <c r="BK9" s="3"/>
-      <c r="BL9" s="3"/>
+      <c r="BL9" s="3">
+        <v>1</v>
+      </c>
       <c r="BM9" s="4"/>
       <c r="BN9" s="4"/>
       <c r="BO9" s="4"/>
@@ -4250,7 +4295,7 @@
       </c>
       <c r="B15" s="11">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C15" s="17">
         <v>1</v>
@@ -4283,17 +4328,39 @@
       <c r="O15" s="3">
         <v>1</v>
       </c>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>1</v>
+      </c>
+      <c r="R15" s="4">
+        <v>1</v>
+      </c>
+      <c r="S15" s="4">
+        <v>1</v>
+      </c>
+      <c r="T15" s="4">
+        <v>1</v>
+      </c>
+      <c r="U15" s="4">
+        <v>1</v>
+      </c>
+      <c r="V15" s="4">
+        <v>1</v>
+      </c>
+      <c r="W15" s="4">
+        <v>1</v>
+      </c>
+      <c r="X15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>1</v>
+      </c>
       <c r="AA15" s="18"/>
       <c r="AB15" s="17">
         <v>1</v>
@@ -4404,19 +4471,45 @@
       <c r="BL15" s="3">
         <v>1</v>
       </c>
-      <c r="BM15" s="4"/>
-      <c r="BN15" s="4"/>
-      <c r="BO15" s="4"/>
-      <c r="BP15" s="4"/>
-      <c r="BQ15" s="4"/>
-      <c r="BR15" s="4"/>
-      <c r="BS15" s="4"/>
-      <c r="BT15" s="4"/>
-      <c r="BU15" s="4"/>
-      <c r="BV15" s="4"/>
-      <c r="BW15" s="4"/>
-      <c r="BX15" s="4"/>
-      <c r="BY15" s="18"/>
+      <c r="BM15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BR15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BU15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX15" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY15" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:102" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
@@ -4886,7 +4979,7 @@
       </c>
       <c r="B19" s="11">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C19" s="17">
         <v>1</v>
@@ -4921,17 +5014,35 @@
       <c r="O19" s="3">
         <v>1</v>
       </c>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
+      <c r="P19" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>1</v>
+      </c>
+      <c r="R19" s="4">
+        <v>1</v>
+      </c>
+      <c r="S19" s="4">
+        <v>1</v>
+      </c>
+      <c r="T19" s="4">
+        <v>1</v>
+      </c>
       <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
+      <c r="V19" s="4">
+        <v>1</v>
+      </c>
+      <c r="W19" s="4">
+        <v>1</v>
+      </c>
       <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
+      <c r="Y19" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>1</v>
+      </c>
       <c r="AA19" s="18"/>
       <c r="AB19" s="17">
         <v>1</v>
@@ -5036,18 +5147,36 @@
       <c r="BL19" s="3">
         <v>1</v>
       </c>
-      <c r="BM19" s="4"/>
+      <c r="BM19" s="4">
+        <v>1</v>
+      </c>
       <c r="BN19" s="4"/>
-      <c r="BO19" s="4"/>
-      <c r="BP19" s="4"/>
-      <c r="BQ19" s="4"/>
+      <c r="BO19" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP19" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ19" s="4">
+        <v>1</v>
+      </c>
       <c r="BR19" s="4"/>
-      <c r="BS19" s="4"/>
+      <c r="BS19" s="4">
+        <v>1</v>
+      </c>
       <c r="BT19" s="4"/>
-      <c r="BU19" s="4"/>
-      <c r="BV19" s="4"/>
-      <c r="BW19" s="4"/>
-      <c r="BX19" s="4"/>
+      <c r="BU19" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV19" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW19" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX19" s="4">
+        <v>1</v>
+      </c>
       <c r="BY19" s="18"/>
     </row>
     <row r="20" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -5056,7 +5185,7 @@
       </c>
       <c r="B20" s="11">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C20" s="17">
         <v>1</v>
@@ -5200,18 +5329,28 @@
       <c r="BL20" s="3">
         <v>1</v>
       </c>
-      <c r="BM20" s="4"/>
+      <c r="BM20" s="4">
+        <v>1</v>
+      </c>
       <c r="BN20" s="4"/>
-      <c r="BO20" s="4"/>
+      <c r="BO20" s="4">
+        <v>1</v>
+      </c>
       <c r="BP20" s="4"/>
       <c r="BQ20" s="4"/>
       <c r="BR20" s="4"/>
-      <c r="BS20" s="4"/>
+      <c r="BS20" s="4">
+        <v>1</v>
+      </c>
       <c r="BT20" s="4"/>
       <c r="BU20" s="4"/>
       <c r="BV20" s="4"/>
-      <c r="BW20" s="4"/>
-      <c r="BX20" s="4"/>
+      <c r="BW20" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX20" s="4">
+        <v>1</v>
+      </c>
       <c r="BY20" s="18"/>
     </row>
     <row r="21" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -5220,7 +5359,7 @@
       </c>
       <c r="B21" s="11">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C21" s="17">
         <v>1</v>
@@ -5398,17 +5537,29 @@
       </c>
       <c r="BM21" s="4"/>
       <c r="BN21" s="4"/>
-      <c r="BO21" s="4"/>
+      <c r="BO21" s="4">
+        <v>1</v>
+      </c>
       <c r="BP21" s="4"/>
       <c r="BQ21" s="4"/>
-      <c r="BR21" s="4"/>
-      <c r="BS21" s="4"/>
+      <c r="BR21" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS21" s="4">
+        <v>1</v>
+      </c>
       <c r="BT21" s="4"/>
       <c r="BU21" s="4"/>
       <c r="BV21" s="4"/>
-      <c r="BW21" s="4"/>
-      <c r="BX21" s="4"/>
-      <c r="BY21" s="18"/>
+      <c r="BW21" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX21" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY21" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
@@ -6042,7 +6193,7 @@
       </c>
       <c r="B26" s="11">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="3"/>
@@ -6130,7 +6281,9 @@
       </c>
       <c r="BM26" s="4"/>
       <c r="BN26" s="4"/>
-      <c r="BO26" s="4"/>
+      <c r="BO26" s="4">
+        <v>1</v>
+      </c>
       <c r="BP26" s="4"/>
       <c r="BQ26" s="4"/>
       <c r="BR26" s="4"/>
@@ -6139,8 +6292,12 @@
       <c r="BU26" s="4"/>
       <c r="BV26" s="4"/>
       <c r="BW26" s="4"/>
-      <c r="BX26" s="4"/>
-      <c r="BY26" s="18"/>
+      <c r="BX26" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY26" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
@@ -6148,7 +6305,7 @@
       </c>
       <c r="B27" s="11">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C27" s="17">
         <v>1</v>
@@ -6306,16 +6463,30 @@
       </c>
       <c r="BM27" s="4"/>
       <c r="BN27" s="4"/>
-      <c r="BO27" s="4"/>
-      <c r="BP27" s="4"/>
-      <c r="BQ27" s="4"/>
+      <c r="BO27" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP27" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ27" s="4">
+        <v>1</v>
+      </c>
       <c r="BR27" s="4"/>
-      <c r="BS27" s="4"/>
+      <c r="BS27" s="4">
+        <v>1</v>
+      </c>
       <c r="BT27" s="4"/>
-      <c r="BU27" s="4"/>
+      <c r="BU27" s="4">
+        <v>1</v>
+      </c>
       <c r="BV27" s="4"/>
-      <c r="BW27" s="4"/>
-      <c r="BX27" s="4"/>
+      <c r="BW27" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX27" s="4">
+        <v>1</v>
+      </c>
       <c r="BY27" s="18"/>
     </row>
     <row r="28" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -6420,7 +6591,7 @@
       </c>
       <c r="B29" s="11">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C29" s="17">
         <v>1</v>
@@ -6606,19 +6777,37 @@
       <c r="BL29" s="3">
         <v>1</v>
       </c>
-      <c r="BM29" s="4"/>
-      <c r="BN29" s="4"/>
-      <c r="BO29" s="4"/>
+      <c r="BM29" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN29" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO29" s="4">
+        <v>1</v>
+      </c>
       <c r="BP29" s="4"/>
       <c r="BQ29" s="4"/>
-      <c r="BR29" s="4"/>
-      <c r="BS29" s="4"/>
-      <c r="BT29" s="4"/>
+      <c r="BR29" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS29" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT29" s="4">
+        <v>1</v>
+      </c>
       <c r="BU29" s="4"/>
       <c r="BV29" s="4"/>
-      <c r="BW29" s="4"/>
-      <c r="BX29" s="4"/>
-      <c r="BY29" s="18"/>
+      <c r="BW29" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX29" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY29" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
@@ -6940,7 +7129,7 @@
       </c>
       <c r="B32" s="11">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C32" s="17">
         <v>1</v>
@@ -7080,18 +7269,40 @@
       <c r="BL32" s="3">
         <v>1</v>
       </c>
-      <c r="BM32" s="4"/>
-      <c r="BN32" s="4"/>
-      <c r="BO32" s="4"/>
-      <c r="BP32" s="4"/>
-      <c r="BQ32" s="4"/>
+      <c r="BM32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ32" s="4">
+        <v>1</v>
+      </c>
       <c r="BR32" s="4"/>
-      <c r="BS32" s="4"/>
-      <c r="BT32" s="4"/>
-      <c r="BU32" s="4"/>
-      <c r="BV32" s="4"/>
-      <c r="BW32" s="4"/>
-      <c r="BX32" s="4"/>
+      <c r="BS32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BU32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX32" s="4">
+        <v>1</v>
+      </c>
       <c r="BY32" s="18"/>
     </row>
     <row r="33" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -7204,7 +7415,7 @@
       </c>
       <c r="B34" s="11">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C34" s="17">
         <v>1</v>
@@ -7362,18 +7573,38 @@
       <c r="BL34" s="3">
         <v>1</v>
       </c>
-      <c r="BM34" s="4"/>
-      <c r="BN34" s="4"/>
-      <c r="BO34" s="4"/>
-      <c r="BP34" s="4"/>
-      <c r="BQ34" s="4"/>
+      <c r="BM34" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN34" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO34" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP34" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ34" s="4">
+        <v>1</v>
+      </c>
       <c r="BR34" s="4"/>
-      <c r="BS34" s="4"/>
+      <c r="BS34" s="4">
+        <v>1</v>
+      </c>
       <c r="BT34" s="4"/>
-      <c r="BU34" s="4"/>
-      <c r="BV34" s="4"/>
-      <c r="BW34" s="4"/>
-      <c r="BX34" s="4"/>
+      <c r="BU34" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV34" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW34" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX34" s="4">
+        <v>1</v>
+      </c>
       <c r="BY34" s="18"/>
     </row>
     <row r="35" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -7382,7 +7613,7 @@
       </c>
       <c r="B35" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C35" s="17">
         <v>1</v>
@@ -7447,10 +7678,16 @@
       <c r="BE35" s="3"/>
       <c r="BF35" s="3"/>
       <c r="BG35" s="3"/>
-      <c r="BH35" s="3"/>
+      <c r="BH35" s="3">
+        <v>1</v>
+      </c>
       <c r="BI35" s="3"/>
-      <c r="BJ35" s="3"/>
-      <c r="BK35" s="3"/>
+      <c r="BJ35" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK35" s="3">
+        <v>1</v>
+      </c>
       <c r="BL35" s="3"/>
       <c r="BM35" s="4"/>
       <c r="BN35" s="4"/>
@@ -7472,7 +7709,7 @@
       </c>
       <c r="B36" s="11">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C36" s="17">
         <v>1</v>
@@ -7567,29 +7804,57 @@
       </c>
       <c r="AZ36" s="18"/>
       <c r="BA36" s="17"/>
-      <c r="BB36" s="3"/>
+      <c r="BB36" s="3">
+        <v>1</v>
+      </c>
       <c r="BC36" s="3"/>
       <c r="BD36" s="3"/>
-      <c r="BE36" s="3"/>
-      <c r="BF36" s="3"/>
-      <c r="BG36" s="3"/>
-      <c r="BH36" s="3"/>
+      <c r="BE36" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF36" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG36" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH36" s="3">
+        <v>1</v>
+      </c>
       <c r="BI36" s="3"/>
-      <c r="BJ36" s="3"/>
-      <c r="BK36" s="3"/>
-      <c r="BL36" s="3"/>
+      <c r="BJ36" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK36" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL36" s="3">
+        <v>1</v>
+      </c>
       <c r="BM36" s="4"/>
       <c r="BN36" s="4"/>
-      <c r="BO36" s="4"/>
-      <c r="BP36" s="4"/>
+      <c r="BO36" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP36" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ36" s="4"/>
       <c r="BR36" s="4"/>
-      <c r="BS36" s="4"/>
+      <c r="BS36" s="4">
+        <v>1</v>
+      </c>
       <c r="BT36" s="4"/>
-      <c r="BU36" s="4"/>
+      <c r="BU36" s="4">
+        <v>1</v>
+      </c>
       <c r="BV36" s="4"/>
-      <c r="BW36" s="4"/>
-      <c r="BX36" s="4"/>
+      <c r="BW36" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX36" s="4">
+        <v>1</v>
+      </c>
       <c r="BY36" s="18"/>
     </row>
     <row r="37" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -9416,7 +9681,7 @@
       </c>
       <c r="B49" s="11">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C49" s="17">
         <v>1</v>
@@ -9580,18 +9845,38 @@
       <c r="BL49" s="3">
         <v>1</v>
       </c>
-      <c r="BM49" s="4"/>
-      <c r="BN49" s="4"/>
-      <c r="BO49" s="4"/>
-      <c r="BP49" s="4"/>
-      <c r="BQ49" s="4"/>
+      <c r="BM49" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN49" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO49" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP49" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ49" s="4">
+        <v>1</v>
+      </c>
       <c r="BR49" s="4"/>
-      <c r="BS49" s="4"/>
+      <c r="BS49" s="4">
+        <v>1</v>
+      </c>
       <c r="BT49" s="4"/>
-      <c r="BU49" s="4"/>
-      <c r="BV49" s="4"/>
-      <c r="BW49" s="4"/>
-      <c r="BX49" s="4"/>
+      <c r="BU49" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV49" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW49" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX49" s="4">
+        <v>1</v>
+      </c>
       <c r="BY49" s="18"/>
     </row>
     <row r="50" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -9996,7 +10281,7 @@
       </c>
       <c r="B53" s="11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C53" s="17"/>
       <c r="D53" s="3"/>
@@ -10082,16 +10367,26 @@
       <c r="BL53" s="3"/>
       <c r="BM53" s="4"/>
       <c r="BN53" s="4"/>
-      <c r="BO53" s="4"/>
-      <c r="BP53" s="4"/>
-      <c r="BQ53" s="4"/>
+      <c r="BO53" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP53" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ53" s="4">
+        <v>1</v>
+      </c>
       <c r="BR53" s="4"/>
       <c r="BS53" s="4"/>
       <c r="BT53" s="4"/>
       <c r="BU53" s="4"/>
       <c r="BV53" s="4"/>
-      <c r="BW53" s="4"/>
-      <c r="BX53" s="4"/>
+      <c r="BW53" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX53" s="4">
+        <v>1</v>
+      </c>
       <c r="BY53" s="18"/>
     </row>
     <row r="54" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -10480,7 +10775,7 @@
       </c>
       <c r="B56" s="11">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C56" s="17">
         <v>1</v>
@@ -10648,19 +10943,37 @@
       <c r="BL56" s="3">
         <v>1</v>
       </c>
-      <c r="BM56" s="4"/>
+      <c r="BM56" s="4">
+        <v>1</v>
+      </c>
       <c r="BN56" s="4"/>
-      <c r="BO56" s="4"/>
-      <c r="BP56" s="4"/>
-      <c r="BQ56" s="4"/>
+      <c r="BO56" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP56" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ56" s="4">
+        <v>1</v>
+      </c>
       <c r="BR56" s="4"/>
-      <c r="BS56" s="4"/>
-      <c r="BT56" s="4"/>
+      <c r="BS56" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT56" s="4">
+        <v>1</v>
+      </c>
       <c r="BU56" s="4"/>
       <c r="BV56" s="4"/>
-      <c r="BW56" s="4"/>
-      <c r="BX56" s="4"/>
-      <c r="BY56" s="18"/>
+      <c r="BW56" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX56" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY56" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
@@ -11194,7 +11507,7 @@
       </c>
       <c r="B60" s="11">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C60" s="19">
         <v>1</v>
@@ -11318,7 +11631,9 @@
       <c r="BL60" s="5"/>
       <c r="BM60" s="6"/>
       <c r="BN60" s="6"/>
-      <c r="BO60" s="6"/>
+      <c r="BO60" s="6">
+        <v>1</v>
+      </c>
       <c r="BP60" s="6"/>
       <c r="BQ60" s="6"/>
       <c r="BR60" s="6"/>
@@ -11326,8 +11641,12 @@
       <c r="BT60" s="6"/>
       <c r="BU60" s="6"/>
       <c r="BV60" s="6"/>
-      <c r="BW60" s="6"/>
-      <c r="BX60" s="6"/>
+      <c r="BW60" s="6">
+        <v>1</v>
+      </c>
+      <c r="BX60" s="6">
+        <v>1</v>
+      </c>
       <c r="BY60" s="20"/>
     </row>
     <row r="61" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -11424,7 +11743,7 @@
       </c>
       <c r="B62" s="11">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="3"/>
@@ -11524,18 +11843,38 @@
       <c r="AZ62" s="21">
         <v>1</v>
       </c>
-      <c r="BA62" s="22"/>
-      <c r="BB62" s="7"/>
-      <c r="BC62" s="7"/>
+      <c r="BA62" s="22">
+        <v>1</v>
+      </c>
+      <c r="BB62" s="7">
+        <v>1</v>
+      </c>
+      <c r="BC62" s="7">
+        <v>1</v>
+      </c>
       <c r="BD62" s="7"/>
-      <c r="BE62" s="7"/>
-      <c r="BF62" s="7"/>
-      <c r="BG62" s="7"/>
-      <c r="BH62" s="7"/>
+      <c r="BE62" s="7">
+        <v>1</v>
+      </c>
+      <c r="BF62" s="7">
+        <v>1</v>
+      </c>
+      <c r="BG62" s="7">
+        <v>1</v>
+      </c>
+      <c r="BH62" s="7">
+        <v>1</v>
+      </c>
       <c r="BI62" s="7"/>
-      <c r="BJ62" s="7"/>
-      <c r="BK62" s="7"/>
-      <c r="BL62" s="7"/>
+      <c r="BJ62" s="7">
+        <v>1</v>
+      </c>
+      <c r="BK62" s="7">
+        <v>1</v>
+      </c>
+      <c r="BL62" s="7">
+        <v>1</v>
+      </c>
       <c r="BM62" s="8">
         <v>1</v>
       </c>
@@ -12120,7 +12459,7 @@
       </c>
       <c r="B66" s="11">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C66" s="17">
         <v>1</v>
@@ -12260,17 +12599,31 @@
       </c>
       <c r="BM66" s="4"/>
       <c r="BN66" s="4"/>
-      <c r="BO66" s="4"/>
-      <c r="BP66" s="4"/>
-      <c r="BQ66" s="4"/>
+      <c r="BO66" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP66" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ66" s="4">
+        <v>1</v>
+      </c>
       <c r="BR66" s="4"/>
-      <c r="BS66" s="4"/>
+      <c r="BS66" s="4">
+        <v>1</v>
+      </c>
       <c r="BT66" s="4"/>
-      <c r="BU66" s="4"/>
+      <c r="BU66" s="4">
+        <v>1</v>
+      </c>
       <c r="BV66" s="4"/>
       <c r="BW66" s="4"/>
-      <c r="BX66" s="4"/>
-      <c r="BY66" s="18"/>
+      <c r="BX66" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY66" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="12" t="s">
@@ -12278,7 +12631,7 @@
       </c>
       <c r="B67" s="11">
         <f t="shared" ref="B67:B130" si="1">SUM(C67:CX67)</f>
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C67" s="17">
         <v>1</v>
@@ -12448,18 +12801,32 @@
       <c r="BL67" s="3">
         <v>1</v>
       </c>
-      <c r="BM67" s="4"/>
-      <c r="BN67" s="4"/>
-      <c r="BO67" s="4"/>
+      <c r="BM67" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN67" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO67" s="4">
+        <v>1</v>
+      </c>
       <c r="BP67" s="4"/>
       <c r="BQ67" s="4"/>
       <c r="BR67" s="4"/>
-      <c r="BS67" s="4"/>
-      <c r="BT67" s="4"/>
+      <c r="BS67" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT67" s="4">
+        <v>1</v>
+      </c>
       <c r="BU67" s="4"/>
       <c r="BV67" s="4"/>
-      <c r="BW67" s="4"/>
-      <c r="BX67" s="4"/>
+      <c r="BW67" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX67" s="4">
+        <v>1</v>
+      </c>
       <c r="BY67" s="18"/>
     </row>
     <row r="68" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -12774,7 +13141,7 @@
       </c>
       <c r="B70" s="11">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C70" s="17">
         <v>1</v>
@@ -12941,8 +13308,12 @@
       <c r="BO70" s="4">
         <v>1</v>
       </c>
-      <c r="BP70" s="4"/>
-      <c r="BQ70" s="4"/>
+      <c r="BP70" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ70" s="4">
+        <v>1</v>
+      </c>
       <c r="BR70" s="4"/>
       <c r="BS70" s="4">
         <v>1</v>
@@ -13058,7 +13429,7 @@
       </c>
       <c r="B72" s="11">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C72" s="17">
         <v>1</v>
@@ -13148,18 +13519,34 @@
       <c r="AZ72" s="18">
         <v>1</v>
       </c>
-      <c r="BA72" s="17"/>
-      <c r="BB72" s="3"/>
+      <c r="BA72" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB72" s="3">
+        <v>1</v>
+      </c>
       <c r="BC72" s="3"/>
       <c r="BD72" s="3"/>
-      <c r="BE72" s="3"/>
-      <c r="BF72" s="3"/>
+      <c r="BE72" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF72" s="3">
+        <v>1</v>
+      </c>
       <c r="BG72" s="3"/>
-      <c r="BH72" s="3"/>
+      <c r="BH72" s="3">
+        <v>1</v>
+      </c>
       <c r="BI72" s="3"/>
-      <c r="BJ72" s="3"/>
-      <c r="BK72" s="3"/>
-      <c r="BL72" s="3"/>
+      <c r="BJ72" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK72" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL72" s="3">
+        <v>1</v>
+      </c>
       <c r="BM72" s="4">
         <v>1</v>
       </c>
@@ -13190,7 +13577,7 @@
       </c>
       <c r="B73" s="11">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C73" s="17">
         <v>1</v>
@@ -13311,17 +13698,33 @@
         <v>1</v>
       </c>
       <c r="BA73" s="17"/>
-      <c r="BB73" s="3"/>
+      <c r="BB73" s="3">
+        <v>1</v>
+      </c>
       <c r="BC73" s="3"/>
       <c r="BD73" s="3"/>
-      <c r="BE73" s="3"/>
-      <c r="BF73" s="3"/>
-      <c r="BG73" s="3"/>
-      <c r="BH73" s="3"/>
+      <c r="BE73" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF73" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG73" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH73" s="3">
+        <v>1</v>
+      </c>
       <c r="BI73" s="3"/>
-      <c r="BJ73" s="3"/>
-      <c r="BK73" s="3"/>
-      <c r="BL73" s="3"/>
+      <c r="BJ73" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK73" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL73" s="3">
+        <v>1</v>
+      </c>
       <c r="BM73" s="4"/>
       <c r="BN73" s="4"/>
       <c r="BO73" s="4">
@@ -13574,7 +13977,7 @@
       </c>
       <c r="B75" s="11">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C75" s="17">
         <v>1</v>
@@ -13674,18 +14077,36 @@
       <c r="AZ75" s="18">
         <v>1</v>
       </c>
-      <c r="BA75" s="17"/>
-      <c r="BB75" s="3"/>
+      <c r="BA75" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB75" s="3">
+        <v>1</v>
+      </c>
       <c r="BC75" s="3"/>
       <c r="BD75" s="3"/>
-      <c r="BE75" s="3"/>
-      <c r="BF75" s="3"/>
-      <c r="BG75" s="3"/>
-      <c r="BH75" s="3"/>
+      <c r="BE75" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF75" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG75" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH75" s="3">
+        <v>1</v>
+      </c>
       <c r="BI75" s="3"/>
-      <c r="BJ75" s="3"/>
-      <c r="BK75" s="3"/>
-      <c r="BL75" s="3"/>
+      <c r="BJ75" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK75" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL75" s="3">
+        <v>1</v>
+      </c>
       <c r="BM75" s="4">
         <v>1</v>
       </c>
@@ -15448,7 +15869,7 @@
       </c>
       <c r="B86" s="11">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C86" s="17"/>
       <c r="D86" s="3"/>
@@ -15528,7 +15949,9 @@
       <c r="BL86" s="3"/>
       <c r="BM86" s="4"/>
       <c r="BN86" s="4"/>
-      <c r="BO86" s="4"/>
+      <c r="BO86" s="4">
+        <v>1</v>
+      </c>
       <c r="BP86" s="4"/>
       <c r="BQ86" s="4"/>
       <c r="BR86" s="4"/>
@@ -15536,8 +15959,12 @@
       <c r="BT86" s="4"/>
       <c r="BU86" s="4"/>
       <c r="BV86" s="4"/>
-      <c r="BW86" s="4"/>
-      <c r="BX86" s="4"/>
+      <c r="BW86" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX86" s="4">
+        <v>1</v>
+      </c>
       <c r="BY86" s="18"/>
     </row>
     <row r="87" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -15804,7 +16231,7 @@
       </c>
       <c r="B89" s="11">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C89" s="17">
         <v>1</v>
@@ -15926,16 +16353,24 @@
       </c>
       <c r="BM89" s="4"/>
       <c r="BN89" s="4"/>
-      <c r="BO89" s="4"/>
+      <c r="BO89" s="4">
+        <v>1</v>
+      </c>
       <c r="BP89" s="4"/>
-      <c r="BQ89" s="4"/>
+      <c r="BQ89" s="4">
+        <v>1</v>
+      </c>
       <c r="BR89" s="4"/>
       <c r="BS89" s="4"/>
       <c r="BT89" s="4"/>
       <c r="BU89" s="4"/>
       <c r="BV89" s="4"/>
-      <c r="BW89" s="4"/>
-      <c r="BX89" s="4"/>
+      <c r="BW89" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX89" s="4">
+        <v>1</v>
+      </c>
       <c r="BY89" s="18"/>
     </row>
     <row r="90" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -16178,7 +16613,7 @@
       </c>
       <c r="B91" s="11">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C91" s="17"/>
       <c r="D91" s="3"/>
@@ -16326,18 +16761,34 @@
       <c r="BL91" s="3">
         <v>1</v>
       </c>
-      <c r="BM91" s="4"/>
-      <c r="BN91" s="4"/>
-      <c r="BO91" s="4"/>
-      <c r="BP91" s="4"/>
-      <c r="BQ91" s="4"/>
+      <c r="BM91" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN91" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO91" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP91" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ91" s="4">
+        <v>1</v>
+      </c>
       <c r="BR91" s="4"/>
-      <c r="BS91" s="4"/>
+      <c r="BS91" s="4">
+        <v>1</v>
+      </c>
       <c r="BT91" s="4"/>
       <c r="BU91" s="4"/>
       <c r="BV91" s="4"/>
-      <c r="BW91" s="4"/>
-      <c r="BX91" s="4"/>
+      <c r="BW91" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX91" s="4">
+        <v>1</v>
+      </c>
       <c r="BY91" s="18"/>
     </row>
     <row r="92" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -16346,7 +16797,7 @@
       </c>
       <c r="B92" s="11">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C92" s="17">
         <v>1</v>
@@ -16466,18 +16917,32 @@
       <c r="BJ92" s="3"/>
       <c r="BK92" s="3"/>
       <c r="BL92" s="3"/>
-      <c r="BM92" s="4"/>
+      <c r="BM92" s="4">
+        <v>1</v>
+      </c>
       <c r="BN92" s="4"/>
-      <c r="BO92" s="4"/>
-      <c r="BP92" s="4"/>
-      <c r="BQ92" s="4"/>
+      <c r="BO92" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP92" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ92" s="4">
+        <v>1</v>
+      </c>
       <c r="BR92" s="4"/>
-      <c r="BS92" s="4"/>
+      <c r="BS92" s="4">
+        <v>1</v>
+      </c>
       <c r="BT92" s="4"/>
       <c r="BU92" s="4"/>
       <c r="BV92" s="4"/>
-      <c r="BW92" s="4"/>
-      <c r="BX92" s="4"/>
+      <c r="BW92" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX92" s="4">
+        <v>1</v>
+      </c>
       <c r="BY92" s="18"/>
     </row>
     <row r="93" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -16672,7 +17137,7 @@
       </c>
       <c r="B94" s="11">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C94" s="17">
         <v>1</v>
@@ -16772,7 +17237,9 @@
       <c r="AZ94" s="18">
         <v>1</v>
       </c>
-      <c r="BA94" s="17"/>
+      <c r="BA94" s="17">
+        <v>1</v>
+      </c>
       <c r="BB94" s="3">
         <v>1</v>
       </c>
@@ -16799,19 +17266,33 @@
       <c r="BK94" s="3">
         <v>1</v>
       </c>
-      <c r="BL94" s="3"/>
+      <c r="BL94" s="3">
+        <v>1</v>
+      </c>
       <c r="BM94" s="4"/>
       <c r="BN94" s="4"/>
-      <c r="BO94" s="4"/>
-      <c r="BP94" s="4"/>
-      <c r="BQ94" s="4"/>
+      <c r="BO94" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP94" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ94" s="4">
+        <v>1</v>
+      </c>
       <c r="BR94" s="4"/>
-      <c r="BS94" s="4"/>
+      <c r="BS94" s="4">
+        <v>1</v>
+      </c>
       <c r="BT94" s="4"/>
       <c r="BU94" s="4"/>
       <c r="BV94" s="4"/>
-      <c r="BW94" s="4"/>
-      <c r="BX94" s="4"/>
+      <c r="BW94" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX94" s="4">
+        <v>1</v>
+      </c>
       <c r="BY94" s="18"/>
     </row>
     <row r="95" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -16820,7 +17301,7 @@
       </c>
       <c r="B95" s="11">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C95" s="17"/>
       <c r="D95" s="3"/>
@@ -16916,18 +17397,34 @@
       <c r="BL95" s="3">
         <v>1</v>
       </c>
-      <c r="BM95" s="4"/>
+      <c r="BM95" s="4">
+        <v>1</v>
+      </c>
       <c r="BN95" s="4"/>
-      <c r="BO95" s="4"/>
-      <c r="BP95" s="4"/>
-      <c r="BQ95" s="4"/>
+      <c r="BO95" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP95" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ95" s="4">
+        <v>1</v>
+      </c>
       <c r="BR95" s="4"/>
-      <c r="BS95" s="4"/>
+      <c r="BS95" s="4">
+        <v>1</v>
+      </c>
       <c r="BT95" s="4"/>
-      <c r="BU95" s="4"/>
+      <c r="BU95" s="4">
+        <v>1</v>
+      </c>
       <c r="BV95" s="4"/>
-      <c r="BW95" s="4"/>
-      <c r="BX95" s="4"/>
+      <c r="BW95" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX95" s="4">
+        <v>1</v>
+      </c>
       <c r="BY95" s="18"/>
     </row>
     <row r="96" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -18140,7 +18637,7 @@
       </c>
       <c r="B103" s="11">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C103" s="17"/>
       <c r="D103" s="3"/>
@@ -18224,7 +18721,9 @@
       <c r="BL103" s="3"/>
       <c r="BM103" s="4"/>
       <c r="BN103" s="4"/>
-      <c r="BO103" s="4"/>
+      <c r="BO103" s="4">
+        <v>1</v>
+      </c>
       <c r="BP103" s="4"/>
       <c r="BQ103" s="4"/>
       <c r="BR103" s="4"/>
@@ -18232,8 +18731,12 @@
       <c r="BT103" s="4"/>
       <c r="BU103" s="4"/>
       <c r="BV103" s="4"/>
-      <c r="BW103" s="4"/>
-      <c r="BX103" s="4"/>
+      <c r="BW103" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX103" s="4">
+        <v>1</v>
+      </c>
       <c r="BY103" s="18"/>
     </row>
     <row r="104" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -18242,7 +18745,7 @@
       </c>
       <c r="B104" s="11">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C104" s="17">
         <v>1</v>
@@ -18390,17 +18893,33 @@
       </c>
       <c r="BM104" s="4"/>
       <c r="BN104" s="4"/>
-      <c r="BO104" s="4"/>
-      <c r="BP104" s="4"/>
-      <c r="BQ104" s="4"/>
+      <c r="BO104" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP104" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ104" s="4">
+        <v>1</v>
+      </c>
       <c r="BR104" s="4"/>
-      <c r="BS104" s="4"/>
+      <c r="BS104" s="4">
+        <v>1</v>
+      </c>
       <c r="BT104" s="4"/>
-      <c r="BU104" s="4"/>
+      <c r="BU104" s="4">
+        <v>1</v>
+      </c>
       <c r="BV104" s="4"/>
-      <c r="BW104" s="4"/>
-      <c r="BX104" s="4"/>
-      <c r="BY104" s="18"/>
+      <c r="BW104" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX104" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY104" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="12" t="s">
@@ -19022,7 +19541,7 @@
       </c>
       <c r="B110" s="11">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C110" s="17">
         <v>1</v>
@@ -19136,13 +19655,23 @@
       <c r="BB110" s="3"/>
       <c r="BC110" s="3"/>
       <c r="BD110" s="3"/>
-      <c r="BE110" s="3"/>
-      <c r="BF110" s="3"/>
+      <c r="BE110" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF110" s="3">
+        <v>1</v>
+      </c>
       <c r="BG110" s="3"/>
-      <c r="BH110" s="3"/>
+      <c r="BH110" s="3">
+        <v>1</v>
+      </c>
       <c r="BI110" s="3"/>
-      <c r="BJ110" s="3"/>
-      <c r="BK110" s="3"/>
+      <c r="BJ110" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK110" s="3">
+        <v>1</v>
+      </c>
       <c r="BL110" s="3"/>
       <c r="BM110" s="4"/>
       <c r="BN110" s="4"/>
@@ -19164,7 +19693,7 @@
       </c>
       <c r="B111" s="11">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C111" s="17">
         <v>1</v>
@@ -19308,18 +19837,34 @@
       <c r="BL111" s="3">
         <v>1</v>
       </c>
-      <c r="BM111" s="4"/>
+      <c r="BM111" s="4">
+        <v>1</v>
+      </c>
       <c r="BN111" s="4"/>
-      <c r="BO111" s="4"/>
-      <c r="BP111" s="4"/>
-      <c r="BQ111" s="4"/>
+      <c r="BO111" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP111" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ111" s="4">
+        <v>1</v>
+      </c>
       <c r="BR111" s="4"/>
-      <c r="BS111" s="4"/>
+      <c r="BS111" s="4">
+        <v>1</v>
+      </c>
       <c r="BT111" s="4"/>
-      <c r="BU111" s="4"/>
+      <c r="BU111" s="4">
+        <v>1</v>
+      </c>
       <c r="BV111" s="4"/>
-      <c r="BW111" s="4"/>
-      <c r="BX111" s="4"/>
+      <c r="BW111" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX111" s="4">
+        <v>1</v>
+      </c>
       <c r="BY111" s="18"/>
     </row>
     <row r="112" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -19472,7 +20017,7 @@
       </c>
       <c r="B113" s="11">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C113" s="17"/>
       <c r="D113" s="3"/>
@@ -19552,18 +20097,28 @@
       <c r="BJ113" s="3"/>
       <c r="BK113" s="3"/>
       <c r="BL113" s="3"/>
-      <c r="BM113" s="4"/>
+      <c r="BM113" s="4">
+        <v>1</v>
+      </c>
       <c r="BN113" s="4"/>
       <c r="BO113" s="4"/>
-      <c r="BP113" s="4"/>
+      <c r="BP113" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ113" s="4"/>
       <c r="BR113" s="4"/>
-      <c r="BS113" s="4"/>
+      <c r="BS113" s="4">
+        <v>1</v>
+      </c>
       <c r="BT113" s="4"/>
       <c r="BU113" s="4"/>
       <c r="BV113" s="4"/>
-      <c r="BW113" s="4"/>
-      <c r="BX113" s="4"/>
+      <c r="BW113" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX113" s="4">
+        <v>1</v>
+      </c>
       <c r="BY113" s="18"/>
     </row>
     <row r="114" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -19572,7 +20127,7 @@
       </c>
       <c r="B114" s="11">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C114" s="17">
         <v>1</v>
@@ -19712,20 +20267,30 @@
       <c r="BL114" s="3">
         <v>1</v>
       </c>
-      <c r="BM114" s="4"/>
+      <c r="BM114" s="4">
+        <v>1</v>
+      </c>
       <c r="BN114" s="4"/>
       <c r="BO114" s="4">
         <v>1</v>
       </c>
-      <c r="BP114" s="4"/>
-      <c r="BQ114" s="4"/>
+      <c r="BP114" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ114" s="4">
+        <v>1</v>
+      </c>
       <c r="BR114" s="4"/>
       <c r="BS114" s="4">
         <v>1</v>
       </c>
       <c r="BT114" s="4"/>
-      <c r="BU114" s="4"/>
-      <c r="BV114" s="4"/>
+      <c r="BU114" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV114" s="4">
+        <v>1</v>
+      </c>
       <c r="BW114" s="4">
         <v>1</v>
       </c>
@@ -20328,7 +20893,7 @@
       </c>
       <c r="B119" s="11">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C119" s="17">
         <v>1</v>
@@ -20442,26 +21007,52 @@
       <c r="BB119" s="3"/>
       <c r="BC119" s="3"/>
       <c r="BD119" s="3"/>
-      <c r="BE119" s="3"/>
-      <c r="BF119" s="3"/>
+      <c r="BE119" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF119" s="3">
+        <v>1</v>
+      </c>
       <c r="BG119" s="3"/>
-      <c r="BH119" s="3"/>
+      <c r="BH119" s="3">
+        <v>1</v>
+      </c>
       <c r="BI119" s="3"/>
-      <c r="BJ119" s="3"/>
-      <c r="BK119" s="3"/>
-      <c r="BL119" s="3"/>
+      <c r="BJ119" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK119" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL119" s="3">
+        <v>1</v>
+      </c>
       <c r="BM119" s="4"/>
       <c r="BN119" s="4"/>
-      <c r="BO119" s="4"/>
-      <c r="BP119" s="4"/>
-      <c r="BQ119" s="4"/>
+      <c r="BO119" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP119" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ119" s="4">
+        <v>1</v>
+      </c>
       <c r="BR119" s="4"/>
-      <c r="BS119" s="4"/>
+      <c r="BS119" s="4">
+        <v>1</v>
+      </c>
       <c r="BT119" s="4"/>
-      <c r="BU119" s="4"/>
+      <c r="BU119" s="4">
+        <v>1</v>
+      </c>
       <c r="BV119" s="4"/>
-      <c r="BW119" s="4"/>
-      <c r="BX119" s="4"/>
+      <c r="BW119" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX119" s="4">
+        <v>1</v>
+      </c>
       <c r="BY119" s="18"/>
     </row>
     <row r="120" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -20656,7 +21247,7 @@
       </c>
       <c r="B122" s="11">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C122" s="17">
         <v>1</v>
@@ -20808,18 +21399,36 @@
       <c r="BL122" s="3">
         <v>1</v>
       </c>
-      <c r="BM122" s="4"/>
-      <c r="BN122" s="4"/>
-      <c r="BO122" s="4"/>
-      <c r="BP122" s="4"/>
-      <c r="BQ122" s="4"/>
+      <c r="BM122" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN122" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO122" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP122" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ122" s="4">
+        <v>1</v>
+      </c>
       <c r="BR122" s="4"/>
-      <c r="BS122" s="4"/>
+      <c r="BS122" s="4">
+        <v>1</v>
+      </c>
       <c r="BT122" s="4"/>
-      <c r="BU122" s="4"/>
+      <c r="BU122" s="4">
+        <v>1</v>
+      </c>
       <c r="BV122" s="4"/>
-      <c r="BW122" s="4"/>
-      <c r="BX122" s="4"/>
+      <c r="BW122" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX122" s="4">
+        <v>1</v>
+      </c>
       <c r="BY122" s="18"/>
     </row>
     <row r="123" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -21140,7 +21749,7 @@
       </c>
       <c r="B125" s="11">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C125" s="17">
         <v>1</v>
@@ -21242,16 +21851,24 @@
       <c r="BL125" s="3"/>
       <c r="BM125" s="4"/>
       <c r="BN125" s="4"/>
-      <c r="BO125" s="4"/>
-      <c r="BP125" s="4"/>
+      <c r="BO125" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP125" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ125" s="4"/>
       <c r="BR125" s="4"/>
       <c r="BS125" s="4"/>
       <c r="BT125" s="4"/>
       <c r="BU125" s="4"/>
       <c r="BV125" s="4"/>
-      <c r="BW125" s="4"/>
-      <c r="BX125" s="4"/>
+      <c r="BW125" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX125" s="4">
+        <v>1</v>
+      </c>
       <c r="BY125" s="18"/>
     </row>
     <row r="126" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -21836,7 +22453,7 @@
       </c>
       <c r="B130" s="11">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C130" s="17">
         <v>1</v>
@@ -21957,15 +22574,23 @@
       <c r="BM130" s="4"/>
       <c r="BN130" s="4"/>
       <c r="BO130" s="4"/>
-      <c r="BP130" s="4"/>
-      <c r="BQ130" s="4"/>
+      <c r="BP130" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ130" s="4">
+        <v>1</v>
+      </c>
       <c r="BR130" s="4"/>
       <c r="BS130" s="4"/>
       <c r="BT130" s="4"/>
       <c r="BU130" s="4"/>
       <c r="BV130" s="4"/>
-      <c r="BW130" s="4"/>
-      <c r="BX130" s="4"/>
+      <c r="BW130" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX130" s="4">
+        <v>1</v>
+      </c>
       <c r="BY130" s="18"/>
     </row>
     <row r="131" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -21974,7 +22599,7 @@
       </c>
       <c r="B131" s="11">
         <f t="shared" ref="B131:B194" si="2">SUM(C131:CX131)</f>
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C131" s="17">
         <v>1</v>
@@ -22098,18 +22723,32 @@
         <v>1</v>
       </c>
       <c r="BL131" s="3"/>
-      <c r="BM131" s="4"/>
+      <c r="BM131" s="4">
+        <v>1</v>
+      </c>
       <c r="BN131" s="4"/>
-      <c r="BO131" s="4"/>
-      <c r="BP131" s="4"/>
-      <c r="BQ131" s="4"/>
+      <c r="BO131" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP131" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ131" s="4">
+        <v>1</v>
+      </c>
       <c r="BR131" s="4"/>
       <c r="BS131" s="4"/>
       <c r="BT131" s="4"/>
-      <c r="BU131" s="4"/>
+      <c r="BU131" s="4">
+        <v>1</v>
+      </c>
       <c r="BV131" s="4"/>
-      <c r="BW131" s="4"/>
-      <c r="BX131" s="4"/>
+      <c r="BW131" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX131" s="4">
+        <v>1</v>
+      </c>
       <c r="BY131" s="18"/>
     </row>
     <row r="132" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -22118,7 +22757,7 @@
       </c>
       <c r="B132" s="11">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C132" s="17">
         <v>1</v>
@@ -22242,18 +22881,38 @@
       <c r="AZ132" s="18">
         <v>1</v>
       </c>
-      <c r="BA132" s="17"/>
-      <c r="BB132" s="3"/>
-      <c r="BC132" s="3"/>
+      <c r="BA132" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB132" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC132" s="3">
+        <v>1</v>
+      </c>
       <c r="BD132" s="3"/>
-      <c r="BE132" s="3"/>
-      <c r="BF132" s="3"/>
-      <c r="BG132" s="3"/>
-      <c r="BH132" s="3"/>
+      <c r="BE132" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF132" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG132" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH132" s="3">
+        <v>1</v>
+      </c>
       <c r="BI132" s="3"/>
-      <c r="BJ132" s="3"/>
-      <c r="BK132" s="3"/>
-      <c r="BL132" s="3"/>
+      <c r="BJ132" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK132" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL132" s="3">
+        <v>1</v>
+      </c>
       <c r="BM132" s="4">
         <v>1</v>
       </c>
@@ -22292,7 +22951,7 @@
       </c>
       <c r="B133" s="11">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C133" s="17">
         <v>1</v>
@@ -22458,19 +23117,39 @@
       <c r="BL133" s="3">
         <v>1</v>
       </c>
-      <c r="BM133" s="4"/>
-      <c r="BN133" s="4"/>
-      <c r="BO133" s="4"/>
-      <c r="BP133" s="4"/>
-      <c r="BQ133" s="4"/>
+      <c r="BM133" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN133" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO133" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP133" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ133" s="4">
+        <v>1</v>
+      </c>
       <c r="BR133" s="4"/>
-      <c r="BS133" s="4"/>
-      <c r="BT133" s="4"/>
+      <c r="BS133" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT133" s="4">
+        <v>1</v>
+      </c>
       <c r="BU133" s="4"/>
       <c r="BV133" s="4"/>
-      <c r="BW133" s="4"/>
-      <c r="BX133" s="4"/>
-      <c r="BY133" s="18"/>
+      <c r="BW133" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX133" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY133" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="134" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A134" s="12" t="s">
@@ -22844,7 +23523,7 @@
       </c>
       <c r="B137" s="11">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C137" s="17">
         <v>1</v>
@@ -22996,18 +23675,28 @@
       <c r="BL137" s="3">
         <v>1</v>
       </c>
-      <c r="BM137" s="4"/>
+      <c r="BM137" s="4">
+        <v>1</v>
+      </c>
       <c r="BN137" s="4"/>
-      <c r="BO137" s="4"/>
+      <c r="BO137" s="4">
+        <v>1</v>
+      </c>
       <c r="BP137" s="4"/>
       <c r="BQ137" s="4"/>
       <c r="BR137" s="4"/>
-      <c r="BS137" s="4"/>
+      <c r="BS137" s="4">
+        <v>1</v>
+      </c>
       <c r="BT137" s="4"/>
       <c r="BU137" s="4"/>
       <c r="BV137" s="4"/>
-      <c r="BW137" s="4"/>
-      <c r="BX137" s="4"/>
+      <c r="BW137" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX137" s="4">
+        <v>1</v>
+      </c>
       <c r="BY137" s="18"/>
     </row>
     <row r="138" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -23016,7 +23705,7 @@
       </c>
       <c r="B138" s="11">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C138" s="17">
         <v>1</v>
@@ -23146,18 +23835,38 @@
       <c r="AZ138" s="18">
         <v>1</v>
       </c>
-      <c r="BA138" s="17"/>
-      <c r="BB138" s="3"/>
-      <c r="BC138" s="3"/>
+      <c r="BA138" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB138" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC138" s="3">
+        <v>1</v>
+      </c>
       <c r="BD138" s="3"/>
-      <c r="BE138" s="3"/>
-      <c r="BF138" s="3"/>
-      <c r="BG138" s="3"/>
-      <c r="BH138" s="3"/>
+      <c r="BE138" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF138" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG138" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH138" s="3">
+        <v>1</v>
+      </c>
       <c r="BI138" s="3"/>
-      <c r="BJ138" s="3"/>
-      <c r="BK138" s="3"/>
-      <c r="BL138" s="3"/>
+      <c r="BJ138" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK138" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL138" s="3">
+        <v>1</v>
+      </c>
       <c r="BM138" s="4"/>
       <c r="BN138" s="4"/>
       <c r="BO138" s="4"/>
@@ -23746,7 +24455,7 @@
       </c>
       <c r="B143" s="11">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C143" s="17">
         <v>1</v>
@@ -23898,18 +24607,42 @@
       <c r="AZ143" s="18">
         <v>1</v>
       </c>
-      <c r="BA143" s="17"/>
-      <c r="BB143" s="3"/>
-      <c r="BC143" s="3"/>
-      <c r="BD143" s="3"/>
-      <c r="BE143" s="3"/>
-      <c r="BF143" s="3"/>
-      <c r="BG143" s="3"/>
-      <c r="BH143" s="3"/>
-      <c r="BI143" s="3"/>
-      <c r="BJ143" s="3"/>
-      <c r="BK143" s="3"/>
-      <c r="BL143" s="3"/>
+      <c r="BA143" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BD143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BE143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BI143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BJ143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK143" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL143" s="3">
+        <v>1</v>
+      </c>
       <c r="BM143" s="4">
         <v>1</v>
       </c>
@@ -23956,7 +24689,7 @@
       </c>
       <c r="B144" s="11">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C144" s="17">
         <v>1</v>
@@ -24130,18 +24863,38 @@
       <c r="BL144" s="3">
         <v>1</v>
       </c>
-      <c r="BM144" s="4"/>
-      <c r="BN144" s="4"/>
-      <c r="BO144" s="4"/>
-      <c r="BP144" s="4"/>
-      <c r="BQ144" s="4"/>
+      <c r="BM144" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN144" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO144" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP144" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ144" s="4">
+        <v>1</v>
+      </c>
       <c r="BR144" s="4"/>
-      <c r="BS144" s="4"/>
+      <c r="BS144" s="4">
+        <v>1</v>
+      </c>
       <c r="BT144" s="4"/>
-      <c r="BU144" s="4"/>
-      <c r="BV144" s="4"/>
-      <c r="BW144" s="4"/>
-      <c r="BX144" s="4"/>
+      <c r="BU144" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV144" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW144" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX144" s="4">
+        <v>1</v>
+      </c>
       <c r="BY144" s="18"/>
     </row>
     <row r="145" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -24150,7 +24903,7 @@
       </c>
       <c r="B145" s="11">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C145" s="17">
         <v>1</v>
@@ -24233,23 +24986,35 @@
       <c r="BE145" s="3"/>
       <c r="BF145" s="3"/>
       <c r="BG145" s="3"/>
-      <c r="BH145" s="3"/>
+      <c r="BH145" s="3">
+        <v>1</v>
+      </c>
       <c r="BI145" s="3"/>
       <c r="BJ145" s="3"/>
-      <c r="BK145" s="3"/>
+      <c r="BK145" s="3">
+        <v>1</v>
+      </c>
       <c r="BL145" s="3"/>
-      <c r="BM145" s="4"/>
+      <c r="BM145" s="4">
+        <v>1</v>
+      </c>
       <c r="BN145" s="4"/>
       <c r="BO145" s="4"/>
-      <c r="BP145" s="4"/>
+      <c r="BP145" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ145" s="4"/>
       <c r="BR145" s="4"/>
       <c r="BS145" s="4"/>
       <c r="BT145" s="4"/>
       <c r="BU145" s="4"/>
       <c r="BV145" s="4"/>
-      <c r="BW145" s="4"/>
-      <c r="BX145" s="4"/>
+      <c r="BW145" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX145" s="4">
+        <v>1</v>
+      </c>
       <c r="BY145" s="18"/>
     </row>
     <row r="146" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -24582,7 +25347,7 @@
       </c>
       <c r="B148" s="11">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C148" s="17">
         <v>1</v>
@@ -24770,19 +25535,45 @@
       <c r="BL148" s="3">
         <v>1</v>
       </c>
-      <c r="BM148" s="4"/>
-      <c r="BN148" s="4"/>
-      <c r="BO148" s="4"/>
-      <c r="BP148" s="4"/>
-      <c r="BQ148" s="4"/>
-      <c r="BR148" s="4"/>
-      <c r="BS148" s="4"/>
-      <c r="BT148" s="4"/>
-      <c r="BU148" s="4"/>
-      <c r="BV148" s="4"/>
-      <c r="BW148" s="4"/>
-      <c r="BX148" s="4"/>
-      <c r="BY148" s="18"/>
+      <c r="BM148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BR148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BU148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX148" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY148" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="149" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A149" s="12" t="s">
@@ -25332,7 +26123,7 @@
       </c>
       <c r="B152" s="11">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C152" s="17">
         <v>1</v>
@@ -25508,19 +26299,35 @@
       <c r="BL152" s="3">
         <v>1</v>
       </c>
-      <c r="BM152" s="4"/>
-      <c r="BN152" s="4"/>
-      <c r="BO152" s="4"/>
+      <c r="BM152" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN152" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO152" s="4">
+        <v>1</v>
+      </c>
       <c r="BP152" s="4"/>
       <c r="BQ152" s="4"/>
       <c r="BR152" s="4"/>
-      <c r="BS152" s="4"/>
-      <c r="BT152" s="4"/>
+      <c r="BS152" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT152" s="4">
+        <v>1</v>
+      </c>
       <c r="BU152" s="4"/>
       <c r="BV152" s="4"/>
-      <c r="BW152" s="4"/>
-      <c r="BX152" s="4"/>
-      <c r="BY152" s="18"/>
+      <c r="BW152" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX152" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY152" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="153" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A153" s="12" t="s">
@@ -25528,7 +26335,7 @@
       </c>
       <c r="B153" s="11">
         <f t="shared" si="2"/>
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C153" s="17">
         <v>1</v>
@@ -25710,18 +26517,40 @@
       <c r="BL153" s="3">
         <v>1</v>
       </c>
-      <c r="BM153" s="4"/>
-      <c r="BN153" s="4"/>
-      <c r="BO153" s="4"/>
-      <c r="BP153" s="4"/>
-      <c r="BQ153" s="4"/>
-      <c r="BR153" s="4"/>
-      <c r="BS153" s="4"/>
+      <c r="BM153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BR153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS153" s="4">
+        <v>1</v>
+      </c>
       <c r="BT153" s="4"/>
-      <c r="BU153" s="4"/>
-      <c r="BV153" s="4"/>
-      <c r="BW153" s="4"/>
-      <c r="BX153" s="4"/>
+      <c r="BU153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW153" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX153" s="4">
+        <v>1</v>
+      </c>
       <c r="BY153" s="18"/>
     </row>
     <row r="154" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -26150,7 +26979,7 @@
       </c>
       <c r="B157" s="11">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C157" s="17">
         <v>1</v>
@@ -26338,19 +27167,43 @@
       <c r="BL157" s="3">
         <v>1</v>
       </c>
-      <c r="BM157" s="4"/>
-      <c r="BN157" s="4"/>
-      <c r="BO157" s="4"/>
+      <c r="BM157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO157" s="4">
+        <v>1</v>
+      </c>
       <c r="BP157" s="4"/>
-      <c r="BQ157" s="4"/>
-      <c r="BR157" s="4"/>
-      <c r="BS157" s="4"/>
-      <c r="BT157" s="4"/>
-      <c r="BU157" s="4"/>
-      <c r="BV157" s="4"/>
-      <c r="BW157" s="4"/>
-      <c r="BX157" s="4"/>
-      <c r="BY157" s="18"/>
+      <c r="BQ157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BR157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BU157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX157" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY157" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A158" s="12" t="s">
@@ -26358,7 +27211,7 @@
       </c>
       <c r="B158" s="11">
         <f t="shared" si="2"/>
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C158" s="17">
         <v>1</v>
@@ -26544,19 +27397,37 @@
       <c r="BL158" s="3">
         <v>1</v>
       </c>
-      <c r="BM158" s="4"/>
-      <c r="BN158" s="4"/>
-      <c r="BO158" s="4"/>
+      <c r="BM158" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN158" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO158" s="4">
+        <v>1</v>
+      </c>
       <c r="BP158" s="4"/>
       <c r="BQ158" s="4"/>
-      <c r="BR158" s="4"/>
-      <c r="BS158" s="4"/>
-      <c r="BT158" s="4"/>
+      <c r="BR158" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS158" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT158" s="4">
+        <v>1</v>
+      </c>
       <c r="BU158" s="4"/>
       <c r="BV158" s="4"/>
-      <c r="BW158" s="4"/>
-      <c r="BX158" s="4"/>
-      <c r="BY158" s="18"/>
+      <c r="BW158" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX158" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY158" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="159" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A159" s="12" t="s">
@@ -27118,7 +27989,7 @@
       </c>
       <c r="B162" s="11">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C162" s="17">
         <v>1</v>
@@ -27283,8 +28154,12 @@
       <c r="BO162" s="4">
         <v>1</v>
       </c>
-      <c r="BP162" s="4"/>
-      <c r="BQ162" s="4"/>
+      <c r="BP162" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ162" s="4">
+        <v>1</v>
+      </c>
       <c r="BR162" s="4"/>
       <c r="BS162" s="4">
         <v>1</v>
@@ -27482,7 +28357,7 @@
       </c>
       <c r="B164" s="11">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C164" s="17">
         <v>1</v>
@@ -27612,19 +28487,35 @@
       <c r="BL164" s="3">
         <v>1</v>
       </c>
-      <c r="BM164" s="4"/>
-      <c r="BN164" s="4"/>
-      <c r="BO164" s="4"/>
+      <c r="BM164" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN164" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO164" s="4">
+        <v>1</v>
+      </c>
       <c r="BP164" s="4"/>
       <c r="BQ164" s="4"/>
       <c r="BR164" s="4"/>
-      <c r="BS164" s="4"/>
-      <c r="BT164" s="4"/>
+      <c r="BS164" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT164" s="4">
+        <v>1</v>
+      </c>
       <c r="BU164" s="4"/>
       <c r="BV164" s="4"/>
-      <c r="BW164" s="4"/>
-      <c r="BX164" s="4"/>
-      <c r="BY164" s="18"/>
+      <c r="BW164" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX164" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY164" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="165" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A165" s="12" t="s">
@@ -27738,7 +28629,7 @@
       </c>
       <c r="B166" s="11">
         <f t="shared" si="2"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C166" s="17">
         <v>1</v>
@@ -27891,7 +28782,9 @@
       <c r="BG166" s="3"/>
       <c r="BH166" s="3"/>
       <c r="BI166" s="3"/>
-      <c r="BJ166" s="3"/>
+      <c r="BJ166" s="3">
+        <v>1</v>
+      </c>
       <c r="BK166" s="3"/>
       <c r="BL166" s="3"/>
       <c r="BM166" s="4">
@@ -28112,7 +29005,7 @@
       </c>
       <c r="B168" s="11">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C168" s="17">
         <v>1</v>
@@ -28254,18 +29147,36 @@
       <c r="BL168" s="3">
         <v>1</v>
       </c>
-      <c r="BM168" s="4"/>
-      <c r="BN168" s="4"/>
-      <c r="BO168" s="4"/>
-      <c r="BP168" s="4"/>
-      <c r="BQ168" s="4"/>
+      <c r="BM168" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN168" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO168" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP168" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ168" s="4">
+        <v>1</v>
+      </c>
       <c r="BR168" s="4"/>
-      <c r="BS168" s="4"/>
+      <c r="BS168" s="4">
+        <v>1</v>
+      </c>
       <c r="BT168" s="4"/>
-      <c r="BU168" s="4"/>
+      <c r="BU168" s="4">
+        <v>1</v>
+      </c>
       <c r="BV168" s="4"/>
-      <c r="BW168" s="4"/>
-      <c r="BX168" s="4"/>
+      <c r="BW168" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX168" s="4">
+        <v>1</v>
+      </c>
       <c r="BY168" s="18"/>
     </row>
     <row r="169" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -28274,7 +29185,7 @@
       </c>
       <c r="B169" s="11">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C169" s="17">
         <v>1</v>
@@ -28381,15 +29292,21 @@
       <c r="BM169" s="4"/>
       <c r="BN169" s="4"/>
       <c r="BO169" s="4"/>
-      <c r="BP169" s="4"/>
-      <c r="BQ169" s="4"/>
+      <c r="BP169" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ169" s="4">
+        <v>1</v>
+      </c>
       <c r="BR169" s="4"/>
       <c r="BS169" s="4"/>
       <c r="BT169" s="4"/>
       <c r="BU169" s="4"/>
       <c r="BV169" s="4"/>
       <c r="BW169" s="4"/>
-      <c r="BX169" s="4"/>
+      <c r="BX169" s="4">
+        <v>1</v>
+      </c>
       <c r="BY169" s="18"/>
     </row>
     <row r="170" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -28592,7 +29509,7 @@
       </c>
       <c r="B171" s="11">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C171" s="17">
         <v>1</v>
@@ -28710,30 +29627,64 @@
       <c r="AZ171" s="18">
         <v>1</v>
       </c>
-      <c r="BA171" s="17"/>
-      <c r="BB171" s="3"/>
+      <c r="BA171" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB171" s="3">
+        <v>1</v>
+      </c>
       <c r="BC171" s="3"/>
       <c r="BD171" s="3"/>
-      <c r="BE171" s="3"/>
-      <c r="BF171" s="3"/>
+      <c r="BE171" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="BF171" s="3">
+        <v>1</v>
+      </c>
       <c r="BG171" s="3"/>
-      <c r="BH171" s="3"/>
+      <c r="BH171" s="3">
+        <v>1</v>
+      </c>
       <c r="BI171" s="3"/>
-      <c r="BJ171" s="3"/>
-      <c r="BK171" s="3"/>
-      <c r="BL171" s="3"/>
-      <c r="BM171" s="4"/>
-      <c r="BN171" s="4"/>
-      <c r="BO171" s="4"/>
-      <c r="BP171" s="4"/>
-      <c r="BQ171" s="4"/>
+      <c r="BJ171" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK171" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL171" s="3">
+        <v>1</v>
+      </c>
+      <c r="BM171" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN171" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO171" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP171" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ171" s="4">
+        <v>1</v>
+      </c>
       <c r="BR171" s="4"/>
-      <c r="BS171" s="4"/>
+      <c r="BS171" s="4">
+        <v>1</v>
+      </c>
       <c r="BT171" s="4"/>
       <c r="BU171" s="4"/>
-      <c r="BV171" s="4"/>
-      <c r="BW171" s="4"/>
-      <c r="BX171" s="4"/>
+      <c r="BV171" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW171" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX171" s="4">
+        <v>1</v>
+      </c>
       <c r="BY171" s="18"/>
     </row>
     <row r="172" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -28742,7 +29693,7 @@
       </c>
       <c r="B172" s="11">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C172" s="17">
         <v>1</v>
@@ -28927,28 +29878,42 @@
       <c r="BM172" s="4">
         <v>1</v>
       </c>
-      <c r="BN172" s="4"/>
+      <c r="BN172" s="4">
+        <v>1</v>
+      </c>
       <c r="BO172" s="4">
         <v>1</v>
       </c>
-      <c r="BP172" s="4"/>
-      <c r="BQ172" s="4"/>
+      <c r="BP172" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ172" s="4">
+        <v>1</v>
+      </c>
       <c r="BR172" s="4">
         <v>1</v>
       </c>
       <c r="BS172" s="4">
         <v>1</v>
       </c>
-      <c r="BT172" s="4"/>
-      <c r="BU172" s="4"/>
-      <c r="BV172" s="4"/>
+      <c r="BT172" s="4">
+        <v>1</v>
+      </c>
+      <c r="BU172" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV172" s="4">
+        <v>1</v>
+      </c>
       <c r="BW172" s="4">
         <v>1</v>
       </c>
       <c r="BX172" s="4">
         <v>1</v>
       </c>
-      <c r="BY172" s="18"/>
+      <c r="BY172" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="173" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A173" s="12" t="s">
@@ -29352,7 +30317,7 @@
       </c>
       <c r="B175" s="11">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C175" s="17">
         <v>1</v>
@@ -29503,8 +30468,12 @@
       <c r="BO175" s="4">
         <v>1</v>
       </c>
-      <c r="BP175" s="4"/>
-      <c r="BQ175" s="4"/>
+      <c r="BP175" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ175" s="4">
+        <v>1</v>
+      </c>
       <c r="BR175" s="4"/>
       <c r="BS175" s="4">
         <v>1</v>
@@ -29526,7 +30495,7 @@
       </c>
       <c r="B176" s="11">
         <f t="shared" si="2"/>
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C176" s="17">
         <v>1</v>
@@ -29662,18 +30631,38 @@
       <c r="AZ176" s="18">
         <v>1</v>
       </c>
-      <c r="BA176" s="17"/>
-      <c r="BB176" s="3"/>
-      <c r="BC176" s="3"/>
+      <c r="BA176" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB176" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC176" s="3">
+        <v>1</v>
+      </c>
       <c r="BD176" s="3"/>
-      <c r="BE176" s="3"/>
-      <c r="BF176" s="3"/>
-      <c r="BG176" s="3"/>
-      <c r="BH176" s="3"/>
+      <c r="BE176" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF176" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG176" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH176" s="3">
+        <v>1</v>
+      </c>
       <c r="BI176" s="3"/>
-      <c r="BJ176" s="3"/>
-      <c r="BK176" s="3"/>
-      <c r="BL176" s="3"/>
+      <c r="BJ176" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK176" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL176" s="3">
+        <v>1</v>
+      </c>
       <c r="BM176" s="4">
         <v>1</v>
       </c>
@@ -29708,7 +30697,9 @@
       <c r="BX176" s="4">
         <v>1</v>
       </c>
-      <c r="BY176" s="18"/>
+      <c r="BY176" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="177" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A177" s="12" t="s">
@@ -30080,7 +31071,7 @@
       </c>
       <c r="B179" s="11">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C179" s="17">
         <v>1</v>
@@ -30246,18 +31237,38 @@
       <c r="BL179" s="7">
         <v>1</v>
       </c>
-      <c r="BM179" s="8"/>
-      <c r="BN179" s="8"/>
-      <c r="BO179" s="8"/>
-      <c r="BP179" s="8"/>
-      <c r="BQ179" s="8"/>
-      <c r="BR179" s="8"/>
-      <c r="BS179" s="8"/>
+      <c r="BM179" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN179" s="8">
+        <v>1</v>
+      </c>
+      <c r="BO179" s="8">
+        <v>1</v>
+      </c>
+      <c r="BP179" s="8">
+        <v>1</v>
+      </c>
+      <c r="BQ179" s="8">
+        <v>1</v>
+      </c>
+      <c r="BR179" s="8">
+        <v>1</v>
+      </c>
+      <c r="BS179" s="8">
+        <v>1</v>
+      </c>
       <c r="BT179" s="8"/>
-      <c r="BU179" s="8"/>
-      <c r="BV179" s="8"/>
+      <c r="BU179" s="8">
+        <v>1</v>
+      </c>
+      <c r="BV179" s="8">
+        <v>1</v>
+      </c>
       <c r="BW179" s="8"/>
-      <c r="BX179" s="8"/>
+      <c r="BX179" s="8">
+        <v>1</v>
+      </c>
       <c r="BY179" s="21"/>
     </row>
     <row r="180" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -30400,7 +31411,7 @@
       </c>
       <c r="B181" s="11">
         <f t="shared" si="2"/>
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C181" s="17">
         <v>1</v>
@@ -30570,19 +31581,43 @@
       <c r="BL181" s="3">
         <v>1</v>
       </c>
-      <c r="BM181" s="4"/>
-      <c r="BN181" s="4"/>
-      <c r="BO181" s="4"/>
-      <c r="BP181" s="4"/>
-      <c r="BQ181" s="4"/>
+      <c r="BM181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ181" s="4">
+        <v>1</v>
+      </c>
       <c r="BR181" s="4"/>
-      <c r="BS181" s="4"/>
-      <c r="BT181" s="4"/>
-      <c r="BU181" s="4"/>
-      <c r="BV181" s="4"/>
-      <c r="BW181" s="4"/>
-      <c r="BX181" s="4"/>
-      <c r="BY181" s="18"/>
+      <c r="BS181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BU181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX181" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY181" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="182" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A182" s="12" t="s">
@@ -30590,7 +31625,7 @@
       </c>
       <c r="B182" s="11">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C182" s="17">
         <v>1</v>
@@ -30742,18 +31777,36 @@
       <c r="BL182" s="3">
         <v>1</v>
       </c>
-      <c r="BM182" s="4"/>
-      <c r="BN182" s="4"/>
-      <c r="BO182" s="4"/>
-      <c r="BP182" s="4"/>
-      <c r="BQ182" s="4"/>
+      <c r="BM182" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN182" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO182" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP182" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ182" s="4">
+        <v>1</v>
+      </c>
       <c r="BR182" s="4"/>
-      <c r="BS182" s="4"/>
+      <c r="BS182" s="4">
+        <v>1</v>
+      </c>
       <c r="BT182" s="4"/>
-      <c r="BU182" s="4"/>
+      <c r="BU182" s="4">
+        <v>1</v>
+      </c>
       <c r="BV182" s="4"/>
-      <c r="BW182" s="4"/>
-      <c r="BX182" s="4"/>
+      <c r="BW182" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX182" s="4">
+        <v>1</v>
+      </c>
       <c r="BY182" s="18"/>
     </row>
     <row r="183" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -30762,7 +31815,7 @@
       </c>
       <c r="B183" s="11">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C183" s="17"/>
       <c r="D183" s="3"/>
@@ -30830,18 +31883,32 @@
       <c r="AZ183" s="18">
         <v>1</v>
       </c>
-      <c r="BA183" s="17"/>
-      <c r="BB183" s="3"/>
+      <c r="BA183" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB183" s="3">
+        <v>1</v>
+      </c>
       <c r="BC183" s="3"/>
       <c r="BD183" s="3"/>
-      <c r="BE183" s="3"/>
+      <c r="BE183" s="3">
+        <v>1</v>
+      </c>
       <c r="BF183" s="3"/>
       <c r="BG183" s="3"/>
-      <c r="BH183" s="3"/>
+      <c r="BH183" s="3">
+        <v>1</v>
+      </c>
       <c r="BI183" s="3"/>
-      <c r="BJ183" s="3"/>
-      <c r="BK183" s="3"/>
-      <c r="BL183" s="3"/>
+      <c r="BJ183" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK183" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL183" s="3">
+        <v>1</v>
+      </c>
       <c r="BM183" s="4"/>
       <c r="BN183" s="4"/>
       <c r="BO183" s="4">
@@ -31096,7 +32163,7 @@
       </c>
       <c r="B186" s="11">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C186" s="17">
         <v>1</v>
@@ -31214,18 +32281,38 @@
       <c r="AZ186" s="18">
         <v>1</v>
       </c>
-      <c r="BA186" s="17"/>
-      <c r="BB186" s="3"/>
-      <c r="BC186" s="3"/>
+      <c r="BA186" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB186" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC186" s="3">
+        <v>1</v>
+      </c>
       <c r="BD186" s="3"/>
-      <c r="BE186" s="3"/>
-      <c r="BF186" s="3"/>
-      <c r="BG186" s="3"/>
-      <c r="BH186" s="3"/>
+      <c r="BE186" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF186" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG186" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH186" s="3">
+        <v>1</v>
+      </c>
       <c r="BI186" s="3"/>
-      <c r="BJ186" s="3"/>
-      <c r="BK186" s="3"/>
-      <c r="BL186" s="3"/>
+      <c r="BJ186" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK186" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL186" s="3">
+        <v>1</v>
+      </c>
       <c r="BM186" s="4">
         <v>1</v>
       </c>
@@ -31928,7 +33015,7 @@
       </c>
       <c r="B192" s="11">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C192" s="17">
         <v>1</v>
@@ -32090,19 +33177,37 @@
       <c r="BL192" s="3">
         <v>1</v>
       </c>
-      <c r="BM192" s="4"/>
+      <c r="BM192" s="4">
+        <v>1</v>
+      </c>
       <c r="BN192" s="4"/>
-      <c r="BO192" s="4"/>
-      <c r="BP192" s="4"/>
-      <c r="BQ192" s="4"/>
+      <c r="BO192" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP192" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ192" s="4">
+        <v>1</v>
+      </c>
       <c r="BR192" s="4"/>
-      <c r="BS192" s="4"/>
+      <c r="BS192" s="4">
+        <v>1</v>
+      </c>
       <c r="BT192" s="4"/>
       <c r="BU192" s="4"/>
-      <c r="BV192" s="4"/>
-      <c r="BW192" s="4"/>
-      <c r="BX192" s="4"/>
-      <c r="BY192" s="18"/>
+      <c r="BV192" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW192" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX192" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY192" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="193" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A193" s="12" t="s">
@@ -32110,7 +33215,7 @@
       </c>
       <c r="B193" s="11">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C193" s="17">
         <v>1</v>
@@ -32214,7 +33319,9 @@
       <c r="AZ193" s="18">
         <v>1</v>
       </c>
-      <c r="BA193" s="17"/>
+      <c r="BA193" s="17">
+        <v>1</v>
+      </c>
       <c r="BB193" s="3">
         <v>1</v>
       </c>
@@ -32226,7 +33333,9 @@
       <c r="BF193" s="3">
         <v>1</v>
       </c>
-      <c r="BG193" s="3"/>
+      <c r="BG193" s="3">
+        <v>1</v>
+      </c>
       <c r="BH193" s="3">
         <v>1</v>
       </c>
@@ -32600,7 +33709,7 @@
       </c>
       <c r="B196" s="11">
         <f t="shared" si="3"/>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C196" s="17">
         <v>1</v>
@@ -32722,7 +33831,9 @@
       <c r="AZ196" s="18">
         <v>1</v>
       </c>
-      <c r="BA196" s="17"/>
+      <c r="BA196" s="17">
+        <v>1</v>
+      </c>
       <c r="BB196" s="3">
         <v>1</v>
       </c>
@@ -33290,7 +34401,7 @@
       </c>
       <c r="B201" s="11">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C201" s="17">
         <v>1</v>
@@ -33420,16 +34531,26 @@
       </c>
       <c r="BM201" s="4"/>
       <c r="BN201" s="4"/>
-      <c r="BO201" s="4"/>
-      <c r="BP201" s="4"/>
+      <c r="BO201" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP201" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ201" s="4"/>
       <c r="BR201" s="4"/>
-      <c r="BS201" s="4"/>
+      <c r="BS201" s="4">
+        <v>1</v>
+      </c>
       <c r="BT201" s="4"/>
       <c r="BU201" s="4"/>
       <c r="BV201" s="4"/>
-      <c r="BW201" s="4"/>
-      <c r="BX201" s="4"/>
+      <c r="BW201" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX201" s="4">
+        <v>1</v>
+      </c>
       <c r="BY201" s="18"/>
     </row>
     <row r="202" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -33438,7 +34559,7 @@
       </c>
       <c r="B202" s="11">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C202" s="17">
         <v>1</v>
@@ -33591,14 +34712,20 @@
       <c r="BO202" s="4">
         <v>1</v>
       </c>
-      <c r="BP202" s="4"/>
-      <c r="BQ202" s="4"/>
+      <c r="BP202" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ202" s="4">
+        <v>1</v>
+      </c>
       <c r="BR202" s="4"/>
       <c r="BS202" s="4">
         <v>1</v>
       </c>
       <c r="BT202" s="4"/>
-      <c r="BU202" s="4"/>
+      <c r="BU202" s="4">
+        <v>1</v>
+      </c>
       <c r="BV202" s="4"/>
       <c r="BW202" s="4">
         <v>1</v>
@@ -34666,7 +35793,7 @@
       </c>
       <c r="B210" s="11">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C210" s="17">
         <v>1</v>
@@ -34804,18 +35931,32 @@
       <c r="BL210" s="3">
         <v>1</v>
       </c>
-      <c r="BM210" s="4"/>
+      <c r="BM210" s="4">
+        <v>1</v>
+      </c>
       <c r="BN210" s="4"/>
-      <c r="BO210" s="4"/>
-      <c r="BP210" s="4"/>
-      <c r="BQ210" s="4"/>
+      <c r="BO210" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP210" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ210" s="4">
+        <v>1</v>
+      </c>
       <c r="BR210" s="4"/>
       <c r="BS210" s="4"/>
       <c r="BT210" s="4"/>
-      <c r="BU210" s="4"/>
+      <c r="BU210" s="4">
+        <v>1</v>
+      </c>
       <c r="BV210" s="4"/>
-      <c r="BW210" s="4"/>
-      <c r="BX210" s="4"/>
+      <c r="BW210" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX210" s="4">
+        <v>1</v>
+      </c>
       <c r="BY210" s="18"/>
     </row>
     <row r="211" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -34824,7 +35965,7 @@
       </c>
       <c r="B211" s="11">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C211" s="17">
         <v>1</v>
@@ -34948,18 +36089,34 @@
       <c r="BL211" s="3">
         <v>1</v>
       </c>
-      <c r="BM211" s="4"/>
-      <c r="BN211" s="4"/>
-      <c r="BO211" s="4"/>
-      <c r="BP211" s="4"/>
-      <c r="BQ211" s="4"/>
+      <c r="BM211" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN211" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO211" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP211" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ211" s="4">
+        <v>1</v>
+      </c>
       <c r="BR211" s="4"/>
-      <c r="BS211" s="4"/>
+      <c r="BS211" s="4">
+        <v>1</v>
+      </c>
       <c r="BT211" s="4"/>
       <c r="BU211" s="4"/>
       <c r="BV211" s="4"/>
-      <c r="BW211" s="4"/>
-      <c r="BX211" s="4"/>
+      <c r="BW211" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX211" s="4">
+        <v>1</v>
+      </c>
       <c r="BY211" s="18"/>
     </row>
     <row r="212" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -35416,7 +36573,7 @@
       </c>
       <c r="B215" s="11">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C215" s="17"/>
       <c r="D215" s="3"/>
@@ -35499,15 +36656,21 @@
       <c r="BM215" s="4"/>
       <c r="BN215" s="4"/>
       <c r="BO215" s="4"/>
-      <c r="BP215" s="4"/>
+      <c r="BP215" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ215" s="4"/>
       <c r="BR215" s="4"/>
       <c r="BS215" s="4"/>
       <c r="BT215" s="4"/>
       <c r="BU215" s="4"/>
       <c r="BV215" s="4"/>
-      <c r="BW215" s="4"/>
-      <c r="BX215" s="4"/>
+      <c r="BW215" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX215" s="4">
+        <v>1</v>
+      </c>
       <c r="BY215" s="18"/>
     </row>
     <row r="216" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -35516,7 +36679,7 @@
       </c>
       <c r="B216" s="11">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C216" s="22">
         <v>1</v>
@@ -35654,17 +36817,25 @@
         <v>1</v>
       </c>
       <c r="BL216" s="3"/>
-      <c r="BM216" s="4"/>
+      <c r="BM216" s="4">
+        <v>1</v>
+      </c>
       <c r="BN216" s="4"/>
       <c r="BO216" s="4">
         <v>1</v>
       </c>
-      <c r="BP216" s="4"/>
-      <c r="BQ216" s="4"/>
+      <c r="BP216" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ216" s="4">
+        <v>1</v>
+      </c>
       <c r="BR216" s="4"/>
       <c r="BS216" s="4"/>
       <c r="BT216" s="4"/>
-      <c r="BU216" s="4"/>
+      <c r="BU216" s="4">
+        <v>1</v>
+      </c>
       <c r="BV216" s="4"/>
       <c r="BW216" s="4">
         <v>1</v>
@@ -35800,7 +36971,7 @@
       </c>
       <c r="B218" s="11">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C218" s="17">
         <v>1</v>
@@ -35960,18 +37131,36 @@
       <c r="BL218" s="3">
         <v>1</v>
       </c>
-      <c r="BM218" s="4"/>
-      <c r="BN218" s="4"/>
-      <c r="BO218" s="4"/>
-      <c r="BP218" s="4"/>
-      <c r="BQ218" s="4"/>
+      <c r="BM218" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN218" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO218" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP218" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ218" s="4">
+        <v>1</v>
+      </c>
       <c r="BR218" s="4"/>
-      <c r="BS218" s="4"/>
+      <c r="BS218" s="4">
+        <v>1</v>
+      </c>
       <c r="BT218" s="4"/>
-      <c r="BU218" s="4"/>
+      <c r="BU218" s="4">
+        <v>1</v>
+      </c>
       <c r="BV218" s="4"/>
-      <c r="BW218" s="4"/>
-      <c r="BX218" s="4"/>
+      <c r="BW218" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX218" s="4">
+        <v>1</v>
+      </c>
       <c r="BY218" s="18"/>
     </row>
     <row r="219" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -36502,7 +37691,7 @@
       </c>
       <c r="B222" s="11">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C222" s="17"/>
       <c r="D222" s="3"/>
@@ -36598,18 +37787,40 @@
       <c r="AZ222" s="18">
         <v>1</v>
       </c>
-      <c r="BA222" s="17"/>
-      <c r="BB222" s="3"/>
-      <c r="BC222" s="3"/>
+      <c r="BA222" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB222" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC222" s="3">
+        <v>1</v>
+      </c>
       <c r="BD222" s="3"/>
-      <c r="BE222" s="3"/>
-      <c r="BF222" s="3"/>
-      <c r="BG222" s="3"/>
-      <c r="BH222" s="3"/>
-      <c r="BI222" s="3"/>
-      <c r="BJ222" s="3"/>
-      <c r="BK222" s="3"/>
-      <c r="BL222" s="3"/>
+      <c r="BE222" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF222" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG222" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH222" s="3">
+        <v>1</v>
+      </c>
+      <c r="BI222" s="3">
+        <v>1</v>
+      </c>
+      <c r="BJ222" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK222" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL222" s="3">
+        <v>1</v>
+      </c>
       <c r="BM222" s="4">
         <v>1</v>
       </c>
@@ -36846,7 +38057,7 @@
       </c>
       <c r="B224" s="11">
         <f t="shared" si="3"/>
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C224" s="17">
         <v>1</v>
@@ -37024,18 +38235,30 @@
       <c r="BL224" s="3">
         <v>1</v>
       </c>
-      <c r="BM224" s="4"/>
+      <c r="BM224" s="4">
+        <v>1</v>
+      </c>
       <c r="BN224" s="4"/>
-      <c r="BO224" s="4"/>
+      <c r="BO224" s="4">
+        <v>1</v>
+      </c>
       <c r="BP224" s="4"/>
       <c r="BQ224" s="4"/>
       <c r="BR224" s="4"/>
-      <c r="BS224" s="4"/>
-      <c r="BT224" s="4"/>
+      <c r="BS224" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT224" s="4">
+        <v>1</v>
+      </c>
       <c r="BU224" s="4"/>
       <c r="BV224" s="4"/>
-      <c r="BW224" s="4"/>
-      <c r="BX224" s="4"/>
+      <c r="BW224" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX224" s="4">
+        <v>1</v>
+      </c>
       <c r="BY224" s="18"/>
     </row>
     <row r="225" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -38042,43 +39265,21 @@
       </c>
       <c r="B230" s="11">
         <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="C230" s="17">
-        <v>1</v>
-      </c>
-      <c r="D230" s="3">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C230" s="17"/>
+      <c r="D230" s="3"/>
       <c r="E230" s="3"/>
-      <c r="F230" s="3">
-        <v>1</v>
-      </c>
-      <c r="G230" s="3">
-        <v>1</v>
-      </c>
+      <c r="F230" s="3"/>
+      <c r="G230" s="3"/>
       <c r="H230" s="3"/>
-      <c r="I230" s="3">
-        <v>1</v>
-      </c>
-      <c r="J230" s="3">
-        <v>1</v>
-      </c>
-      <c r="K230" s="3">
-        <v>1</v>
-      </c>
-      <c r="L230" s="3">
-        <v>1</v>
-      </c>
-      <c r="M230" s="3">
-        <v>1</v>
-      </c>
-      <c r="N230" s="3">
-        <v>1</v>
-      </c>
-      <c r="O230" s="3">
-        <v>1</v>
-      </c>
+      <c r="I230" s="3"/>
+      <c r="J230" s="3"/>
+      <c r="K230" s="3"/>
+      <c r="L230" s="3"/>
+      <c r="M230" s="3"/>
+      <c r="N230" s="3"/>
+      <c r="O230" s="3"/>
       <c r="P230" s="4">
         <v>1</v>
       </c>
@@ -38136,17 +39337,31 @@
       <c r="AZ230" s="18">
         <v>1</v>
       </c>
-      <c r="BA230" s="17"/>
+      <c r="BA230" s="17">
+        <v>1</v>
+      </c>
       <c r="BB230" s="3"/>
       <c r="BC230" s="3"/>
       <c r="BD230" s="3"/>
-      <c r="BE230" s="3"/>
-      <c r="BF230" s="3"/>
-      <c r="BG230" s="3"/>
-      <c r="BH230" s="3"/>
+      <c r="BE230" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF230" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG230" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH230" s="3">
+        <v>1</v>
+      </c>
       <c r="BI230" s="3"/>
-      <c r="BJ230" s="3"/>
-      <c r="BK230" s="3"/>
+      <c r="BJ230" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK230" s="3">
+        <v>1</v>
+      </c>
       <c r="BL230" s="3"/>
       <c r="BM230" s="4"/>
       <c r="BN230" s="4"/>
@@ -38388,7 +39603,7 @@
       </c>
       <c r="B232" s="11">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C232" s="17">
         <v>1</v>
@@ -38556,18 +39771,34 @@
       <c r="BL232" s="3">
         <v>1</v>
       </c>
-      <c r="BM232" s="4"/>
+      <c r="BM232" s="4">
+        <v>1</v>
+      </c>
       <c r="BN232" s="4"/>
-      <c r="BO232" s="4"/>
-      <c r="BP232" s="4"/>
-      <c r="BQ232" s="4"/>
+      <c r="BO232" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP232" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ232" s="4">
+        <v>1</v>
+      </c>
       <c r="BR232" s="4"/>
-      <c r="BS232" s="4"/>
+      <c r="BS232" s="4">
+        <v>1</v>
+      </c>
       <c r="BT232" s="4"/>
       <c r="BU232" s="4"/>
-      <c r="BV232" s="4"/>
-      <c r="BW232" s="4"/>
-      <c r="BX232" s="4"/>
+      <c r="BV232" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW232" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX232" s="4">
+        <v>1</v>
+      </c>
       <c r="BY232" s="18"/>
     </row>
     <row r="233" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
@@ -38576,7 +39807,7 @@
       </c>
       <c r="B233" s="11">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C233" s="17">
         <v>1</v>
@@ -38678,18 +39909,34 @@
       <c r="AZ233" s="18">
         <v>1</v>
       </c>
-      <c r="BA233" s="17"/>
-      <c r="BB233" s="3"/>
+      <c r="BA233" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB233" s="3">
+        <v>1</v>
+      </c>
       <c r="BC233" s="3"/>
       <c r="BD233" s="3"/>
-      <c r="BE233" s="3"/>
-      <c r="BF233" s="3"/>
+      <c r="BE233" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF233" s="3">
+        <v>1</v>
+      </c>
       <c r="BG233" s="3"/>
-      <c r="BH233" s="3"/>
+      <c r="BH233" s="3">
+        <v>1</v>
+      </c>
       <c r="BI233" s="3"/>
-      <c r="BJ233" s="3"/>
-      <c r="BK233" s="3"/>
-      <c r="BL233" s="3"/>
+      <c r="BJ233" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK233" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL233" s="3">
+        <v>1</v>
+      </c>
       <c r="BM233" s="4">
         <v>1</v>
       </c>
@@ -39524,7 +40771,7 @@
       </c>
       <c r="B238" s="11">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C238" s="17">
         <v>1</v>
@@ -39656,18 +40903,40 @@
       <c r="AZ238" s="18">
         <v>1</v>
       </c>
-      <c r="BA238" s="17"/>
-      <c r="BB238" s="3"/>
-      <c r="BC238" s="3"/>
+      <c r="BA238" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB238" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC238" s="3">
+        <v>1</v>
+      </c>
       <c r="BD238" s="3"/>
-      <c r="BE238" s="3"/>
-      <c r="BF238" s="3"/>
-      <c r="BG238" s="3"/>
-      <c r="BH238" s="3"/>
-      <c r="BI238" s="3"/>
-      <c r="BJ238" s="3"/>
-      <c r="BK238" s="3"/>
-      <c r="BL238" s="3"/>
+      <c r="BE238" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF238" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG238" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH238" s="3">
+        <v>1</v>
+      </c>
+      <c r="BI238" s="3">
+        <v>1</v>
+      </c>
+      <c r="BJ238" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK238" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL238" s="3">
+        <v>1</v>
+      </c>
       <c r="BM238" s="4">
         <v>1</v>
       </c>
@@ -39710,7 +40979,7 @@
       </c>
       <c r="B239" s="11">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C239" s="17">
         <v>1</v>
@@ -39870,18 +41139,36 @@
       <c r="BL239" s="3">
         <v>1</v>
       </c>
-      <c r="BM239" s="4"/>
-      <c r="BN239" s="4"/>
-      <c r="BO239" s="4"/>
-      <c r="BP239" s="4"/>
+      <c r="BM239" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN239" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO239" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP239" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ239" s="4"/>
       <c r="BR239" s="4"/>
-      <c r="BS239" s="4"/>
+      <c r="BS239" s="4">
+        <v>1</v>
+      </c>
       <c r="BT239" s="4"/>
-      <c r="BU239" s="4"/>
-      <c r="BV239" s="4"/>
-      <c r="BW239" s="4"/>
-      <c r="BX239" s="4"/>
+      <c r="BU239" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV239" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW239" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX239" s="4">
+        <v>1</v>
+      </c>
       <c r="BY239" s="18"/>
     </row>
     <row r="240" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>